<commit_message>
working on correlation analysis
trying to figure out a way to daisy chain descend a correlation analysis (sorted linked list).  Following a hiearchy from parent to sibling, and then from sibling to next closest relation
</commit_message>
<xml_diff>
--- a/code/Screener/reports/2022-07-15_completed_fred_pvt.xlsx
+++ b/code/Screener/reports/2022-07-15_completed_fred_pvt.xlsx
@@ -886,6 +886,106 @@
     </pic>
     <clientData/>
   </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>1</col>
+      <colOff>0</colOff>
+      <row>487</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="10353675" cy="4838700"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="19" name="Image 19" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId19"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>1</col>
+      <colOff>0</colOff>
+      <row>514</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="10353675" cy="4838700"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="20" name="Image 20" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId20"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>1</col>
+      <colOff>0</colOff>
+      <row>541</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="10353675" cy="4838700"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="21" name="Image 21" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId21"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>1</col>
+      <colOff>0</colOff>
+      <row>568</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="10353675" cy="4838700"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="22" name="Image 22" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId22"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
 </wsDr>
 </file>
 
@@ -1557,7 +1657,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:AE3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1696,6 +1796,31 @@
           <t>name</t>
         </is>
       </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>high_value</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -1708,7 +1833,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2022-07-16 01:24:44</t>
+          <t>2022-07-16 10:23:13</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1731,7 +1856,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>AWHAETP</t>
+          <t>WPU101</t>
         </is>
       </c>
       <c r="I2" t="n">
@@ -1747,7 +1872,7 @@
         <v>222.4253656575287</v>
       </c>
       <c r="M2" t="n">
-        <v>95.08377751526875</v>
+        <v>95.08377751526876</v>
       </c>
       <c r="N2" t="n">
         <v>2</v>
@@ -1774,7 +1899,7 @@
         <v>2</v>
       </c>
       <c r="V2" t="n">
-        <v>8.212685127145461</v>
+        <v>7.128404922900172</v>
       </c>
       <c r="W2" t="n">
         <v>2</v>
@@ -1789,6 +1914,23 @@
         <is>
           <t>PCE</t>
         </is>
+      </c>
+      <c r="AA2" t="n">
+        <v>0.9859267780170259</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0.9859267780170259</v>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>CPIAUCSL</t>
+        </is>
+      </c>
+      <c r="AD2" t="n">
+        <v>0.9859267780170259</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>0.9859267780170259</v>
       </c>
     </row>
     <row r="3">
@@ -1802,7 +1944,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2022-07-16 01:32:29</t>
+          <t>2022-07-16 10:27:01</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1825,7 +1967,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>AWHAETP</t>
+          <t>WPU101</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -1841,7 +1983,7 @@
         <v>222.4253656575287</v>
       </c>
       <c r="M3" t="n">
-        <v>95.08377751526875</v>
+        <v>95.08377751526876</v>
       </c>
       <c r="N3" t="n">
         <v>2</v>
@@ -1868,7 +2010,7 @@
         <v>2</v>
       </c>
       <c r="V3" t="n">
-        <v>8.212685127145461</v>
+        <v>7.128404922900172</v>
       </c>
       <c r="W3" t="n">
         <v>2</v>
@@ -1883,6 +2025,23 @@
         <is>
           <t>PCE</t>
         </is>
+      </c>
+      <c r="AA3" t="n">
+        <v>0.9859267780170259</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>0.9859267780170259</v>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>CPIAUCSL</t>
+        </is>
+      </c>
+      <c r="AD3" t="n">
+        <v>0.9859267780170259</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>0.9859267780170259</v>
       </c>
     </row>
   </sheetData>
@@ -1942,7 +2101,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>EDA</t>
+          <t>fred_data</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1951,7 +2110,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -1960,7 +2119,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2022-07-16 01:24:44</t>
+          <t>2022-07-16 10:23:13</t>
         </is>
       </c>
     </row>
@@ -1988,7 +2147,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2022-07-16 01:32:29</t>
+          <t>2022-07-16 10:27:01</t>
         </is>
       </c>
     </row>
@@ -2120,847 +2279,847 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1488.268166666667</v>
+        <v>1518.70469</v>
       </c>
       <c r="B2" t="n">
-        <v>376.0766666666667</v>
+        <v>396.4766666666667</v>
       </c>
       <c r="C2" t="n">
-        <v>244.12</v>
+        <v>207.3266666666667</v>
       </c>
       <c r="D2" t="n">
-        <v>10.93333333333333</v>
+        <v>22.07</v>
       </c>
       <c r="E2" t="n">
-        <v>3.796666666666666</v>
+        <v>6.933333333333334</v>
       </c>
       <c r="F2" t="n">
-        <v>12.04</v>
+        <v>26.37</v>
       </c>
       <c r="G2" t="n">
-        <v>2247.25593</v>
+        <v>2698.391866666667</v>
       </c>
       <c r="H2" t="n">
-        <v>34.5</v>
+        <v>34.89666666666667</v>
       </c>
       <c r="I2" t="n">
-        <v>98.64999999999999</v>
+        <v>81.75333333333333</v>
       </c>
       <c r="J2" t="n">
-        <v>9.811155195652175</v>
+        <v>9.402214543478262</v>
       </c>
       <c r="K2" t="n">
-        <v>74.63333333333334</v>
+        <v>40.05</v>
       </c>
       <c r="L2" t="n">
-        <v>252.8412333333333</v>
+        <v>260.3466</v>
       </c>
       <c r="M2" t="n">
-        <v>205.3912</v>
+        <v>229.7583333333334</v>
       </c>
       <c r="N2" t="n">
-        <v>2.182</v>
+        <v>0.09</v>
       </c>
       <c r="O2" t="n">
-        <v>0.86</v>
+        <v>0.59</v>
       </c>
       <c r="P2" t="n">
         <v>0</v>
       </c>
       <c r="Q2" t="n">
-        <v>100.2896470386735</v>
+        <v>98.79102009760062</v>
       </c>
       <c r="R2" t="n">
-        <v>125.8326666666667</v>
+        <v>122.8773333333333</v>
       </c>
       <c r="S2" t="n">
-        <v>104.0515633333333</v>
+        <v>96.79987</v>
       </c>
       <c r="T2" t="n">
-        <v>67904.2</v>
+        <v>62779.6</v>
       </c>
       <c r="U2" t="n">
-        <v>14116.63666666667</v>
+        <v>14543.85666666667</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1518.70469</v>
+        <v>1518.463696666667</v>
       </c>
       <c r="B3" t="n">
-        <v>396.4766666666667</v>
+        <v>382.71</v>
       </c>
       <c r="C3" t="n">
-        <v>207.3266666666667</v>
+        <v>200.9866666666667</v>
       </c>
       <c r="D3" t="n">
-        <v>22.07</v>
+        <v>19.65</v>
       </c>
       <c r="E3" t="n">
-        <v>6.933333333333334</v>
+        <v>10.22666666666667</v>
       </c>
       <c r="F3" t="n">
-        <v>26.37</v>
+        <v>30.43</v>
       </c>
       <c r="G3" t="n">
-        <v>2698.391866666667</v>
+        <v>2858.75815</v>
       </c>
       <c r="H3" t="n">
-        <v>34.89666666666667</v>
+        <v>34.6</v>
       </c>
       <c r="I3" t="n">
-        <v>81.75333333333333</v>
+        <v>72.68666666666667</v>
       </c>
       <c r="J3" t="n">
-        <v>9.402214543478262</v>
+        <v>9.193901098901099</v>
       </c>
       <c r="K3" t="n">
-        <v>40.05</v>
+        <v>39.27</v>
       </c>
       <c r="L3" t="n">
-        <v>260.3466</v>
+        <v>258.4988</v>
       </c>
       <c r="M3" t="n">
-        <v>229.7583333333334</v>
+        <v>221.5394333333333</v>
       </c>
       <c r="N3" t="n">
-        <v>0.09</v>
+        <v>0.08966666666666666</v>
       </c>
       <c r="O3" t="n">
-        <v>0.59</v>
+        <v>0.5</v>
       </c>
       <c r="P3" t="n">
         <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>98.79102009760062</v>
+        <v>97.62538150086982</v>
       </c>
       <c r="R3" t="n">
-        <v>122.8773333333333</v>
+        <v>119.739</v>
       </c>
       <c r="S3" t="n">
-        <v>96.79987</v>
+        <v>95.12751333333333</v>
       </c>
       <c r="T3" t="n">
-        <v>62779.6</v>
+        <v>60043.43333333333</v>
       </c>
       <c r="U3" t="n">
-        <v>14543.85666666667</v>
+        <v>14121.20333333333</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1549.487913333333</v>
+        <v>1580.510146666667</v>
       </c>
       <c r="B4" t="n">
-        <v>373.61</v>
+        <v>542.1844333333333</v>
       </c>
       <c r="C4" t="n">
-        <v>217.0866666666667</v>
+        <v>381.8903</v>
       </c>
       <c r="D4" t="n">
-        <v>14.71666666666667</v>
+        <v>15.97</v>
       </c>
       <c r="E4" t="n">
-        <v>3.696666666666667</v>
+        <v>5.416666666666667</v>
       </c>
       <c r="F4" t="n">
-        <v>14.4</v>
+        <v>15.83</v>
       </c>
       <c r="G4" t="n">
-        <v>2343.950213333334</v>
+        <v>2448.47103</v>
       </c>
       <c r="H4" t="n">
-        <v>34.4</v>
+        <v>34.8</v>
       </c>
       <c r="I4" t="n">
-        <v>98.39333333333335</v>
+        <v>81.34333333333333</v>
       </c>
       <c r="J4" t="n">
-        <v>9.939332252747253</v>
+        <v>9.20270443956044</v>
       </c>
       <c r="K4" t="n">
-        <v>58.67333333333333</v>
+        <v>73.52</v>
       </c>
       <c r="L4" t="n">
-        <v>255.8820333333333</v>
+        <v>272.1430333333333</v>
       </c>
       <c r="M4" t="n">
-        <v>211.3559333333333</v>
+        <v>265.4335</v>
       </c>
       <c r="N4" t="n">
-        <v>2.399333333333333</v>
+        <v>0.09933333333333333</v>
       </c>
       <c r="O4" t="n">
-        <v>-0.16</v>
+        <v>1.4</v>
       </c>
       <c r="P4" t="n">
         <v>0</v>
       </c>
       <c r="Q4" t="n">
-        <v>99.32935104420365</v>
+        <v>100.5441661244718</v>
       </c>
       <c r="R4" t="n">
-        <v>128.3126666666667</v>
+        <v>127.9216666666667</v>
       </c>
       <c r="S4" t="n">
-        <v>102.2142533333333</v>
+        <v>100.84973</v>
       </c>
       <c r="T4" t="n">
-        <v>65884.36666666667</v>
+        <v>68643.26666666666</v>
       </c>
       <c r="U4" t="n">
-        <v>14485.34333333333</v>
+        <v>15814.47</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1518.463696666667</v>
+        <v>1471.535181218638</v>
       </c>
       <c r="B5" t="n">
-        <v>382.71</v>
+        <v>398.0820788530465</v>
       </c>
       <c r="C5" t="n">
-        <v>200.9866666666667</v>
+        <v>244.225376344086</v>
       </c>
       <c r="D5" t="n">
-        <v>19.65</v>
+        <v>11.08333333333333</v>
       </c>
       <c r="E5" t="n">
-        <v>10.22666666666667</v>
+        <v>3.808888888888889</v>
       </c>
       <c r="F5" t="n">
-        <v>30.43</v>
+        <v>15.92666666666667</v>
       </c>
       <c r="G5" t="n">
-        <v>2858.75815</v>
+        <v>2200.957183655914</v>
       </c>
       <c r="H5" t="n">
-        <v>34.6</v>
+        <v>34.5</v>
       </c>
       <c r="I5" t="n">
-        <v>72.68666666666667</v>
+        <v>97.89505376344086</v>
       </c>
       <c r="J5" t="n">
-        <v>9.193901098901099</v>
+        <v>9.797889828555501</v>
       </c>
       <c r="K5" t="n">
-        <v>39.27</v>
+        <v>74.05</v>
       </c>
       <c r="L5" t="n">
-        <v>258.4988</v>
+        <v>251.3184695340502</v>
       </c>
       <c r="M5" t="n">
-        <v>221.5394333333333</v>
+        <v>204.9377089605735</v>
       </c>
       <c r="N5" t="n">
-        <v>0.08966666666666666</v>
+        <v>1.906</v>
       </c>
       <c r="O5" t="n">
-        <v>0.5</v>
+        <v>0.91</v>
       </c>
       <c r="P5" t="n">
         <v>0</v>
       </c>
       <c r="Q5" t="n">
-        <v>97.62538150086982</v>
+        <v>100.6185806839007</v>
       </c>
       <c r="R5" t="n">
-        <v>119.739</v>
+        <v>125.0281146953405</v>
       </c>
       <c r="S5" t="n">
-        <v>95.12751333333333</v>
+        <v>103.4573125448029</v>
       </c>
       <c r="T5" t="n">
-        <v>60043.43333333333</v>
+        <v>68361.42939068101</v>
       </c>
       <c r="U5" t="n">
-        <v>14121.20333333333</v>
+        <v>13960.94917562724</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1433.161535483871</v>
+        <v>1665.835980645161</v>
       </c>
       <c r="B6" t="n">
-        <v>410.1193548387097</v>
+        <v>549.6875806451612</v>
       </c>
       <c r="C6" t="n">
-        <v>217.4451612903226</v>
+        <v>423.7149032258064</v>
       </c>
       <c r="D6" t="n">
-        <v>11.46</v>
+        <v>14.61</v>
       </c>
       <c r="E6" t="n">
-        <v>4.006451612903225</v>
+        <v>3.996774193548387</v>
       </c>
       <c r="F6" t="n">
-        <v>10.405</v>
+        <v>17.22</v>
       </c>
       <c r="G6" t="n">
-        <v>2107.725608064516</v>
+        <v>2487.060125806452</v>
       </c>
       <c r="H6" t="n">
-        <v>34.40645161290323</v>
+        <v>34.60645161290323</v>
       </c>
       <c r="I6" t="n">
-        <v>95.7741935483871</v>
+        <v>67.30967741935484</v>
       </c>
       <c r="J6" t="n">
-        <v>9.846498242149758</v>
+        <v>9.516867326086956</v>
       </c>
       <c r="K6" t="n">
-        <v>60.415</v>
+        <v>75.33</v>
       </c>
       <c r="L6" t="n">
-        <v>248.7088387096774</v>
+        <v>281.8747096774193</v>
       </c>
       <c r="M6" t="n">
-        <v>196.1336774193548</v>
+        <v>281.9601290322581</v>
       </c>
       <c r="N6" t="n">
-        <v>1.404838709677419</v>
+        <v>0.08</v>
       </c>
       <c r="O6" t="n">
-        <v>1.015</v>
+        <v>1.46</v>
       </c>
       <c r="P6" t="n">
         <v>0</v>
       </c>
       <c r="Q6" t="n">
-        <v>100.5199462359304</v>
+        <v>100.0793983529852</v>
       </c>
       <c r="R6" t="n">
-        <v>123.0925806451613</v>
+        <v>131.7567741935484</v>
       </c>
       <c r="S6" t="n">
-        <v>101.3529064516129</v>
+        <v>102.1335064516129</v>
       </c>
       <c r="T6" t="n">
-        <v>63835.80645161291</v>
+        <v>72184.16129032258</v>
       </c>
       <c r="U6" t="n">
-        <v>13619.81290322581</v>
+        <v>16533.59032258064</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1407.679989390681</v>
+        <v>1549.487913333333</v>
       </c>
       <c r="B7" t="n">
-        <v>398.6220071684588</v>
+        <v>373.61</v>
       </c>
       <c r="C7" t="n">
-        <v>211.6576344086021</v>
+        <v>217.0866666666667</v>
       </c>
       <c r="D7" t="n">
-        <v>11.75333333333333</v>
+        <v>14.71666666666667</v>
       </c>
       <c r="E7" t="n">
-        <v>4.204444444444444</v>
+        <v>3.696666666666667</v>
       </c>
       <c r="F7" t="n">
-        <v>9.49</v>
+        <v>14.4</v>
       </c>
       <c r="G7" t="n">
-        <v>2111.770228530466</v>
+        <v>2343.950213333334</v>
       </c>
       <c r="H7" t="n">
-        <v>34.39663082437276</v>
+        <v>34.4</v>
       </c>
       <c r="I7" t="n">
-        <v>100.4274551971326</v>
+        <v>98.39333333333335</v>
       </c>
       <c r="J7" t="n">
-        <v>9.913020010869564</v>
+        <v>9.939332252747253</v>
       </c>
       <c r="K7" t="n">
-        <v>51.31</v>
+        <v>58.67333333333333</v>
       </c>
       <c r="L7" t="n">
-        <v>246.6245863799283</v>
+        <v>255.8820333333333</v>
       </c>
       <c r="M7" t="n">
-        <v>195.0992143369176</v>
+        <v>211.3559333333333</v>
       </c>
       <c r="N7" t="n">
-        <v>1.15010752688172</v>
+        <v>2.399333333333333</v>
       </c>
       <c r="O7" t="n">
-        <v>1.29</v>
+        <v>-0.16</v>
       </c>
       <c r="P7" t="n">
         <v>0</v>
       </c>
       <c r="Q7" t="n">
-        <v>100.2700716578218</v>
+        <v>99.32935104420365</v>
       </c>
       <c r="R7" t="n">
-        <v>122.2105663082437</v>
+        <v>128.3126666666667</v>
       </c>
       <c r="S7" t="n">
-        <v>100.9862233691756</v>
+        <v>102.2142533333333</v>
       </c>
       <c r="T7" t="n">
-        <v>63953.99569892474</v>
+        <v>65884.36666666667</v>
       </c>
       <c r="U7" t="n">
-        <v>13394.56494623656</v>
+        <v>14485.34333333333</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1665.835980645161</v>
+        <v>1759.5398</v>
       </c>
       <c r="B8" t="n">
-        <v>549.6875806451612</v>
+        <v>542.649</v>
       </c>
       <c r="C8" t="n">
-        <v>423.7149032258064</v>
+        <v>412.865</v>
       </c>
       <c r="D8" t="n">
-        <v>14.61</v>
+        <v>19.61</v>
       </c>
       <c r="E8" t="n">
-        <v>3.996774193548387</v>
+        <v>3.6</v>
       </c>
       <c r="F8" t="n">
-        <v>17.22</v>
+        <v>28.71</v>
       </c>
       <c r="G8" t="n">
-        <v>2487.060125806452</v>
+        <v>2661.893</v>
       </c>
       <c r="H8" t="n">
-        <v>34.60645161290323</v>
+        <v>34.5</v>
       </c>
       <c r="I8" t="n">
-        <v>67.30967741935484</v>
+        <v>58.85333333333333</v>
       </c>
       <c r="J8" t="n">
         <v>9.516867326086956</v>
       </c>
       <c r="K8" t="n">
-        <v>75.33</v>
+        <v>107.76</v>
       </c>
       <c r="L8" t="n">
-        <v>281.8747096774193</v>
+        <v>295.328</v>
       </c>
       <c r="M8" t="n">
-        <v>281.9601290322581</v>
+        <v>300.845</v>
       </c>
       <c r="N8" t="n">
-        <v>0.08</v>
+        <v>1.21</v>
       </c>
       <c r="O8" t="n">
-        <v>1.46</v>
+        <v>1.26</v>
       </c>
       <c r="P8" t="n">
         <v>0</v>
       </c>
       <c r="Q8" t="n">
-        <v>100.0793983529852</v>
+        <v>99.4414473129178</v>
       </c>
       <c r="R8" t="n">
-        <v>131.7567741935484</v>
+        <v>134.1606666666667</v>
       </c>
       <c r="S8" t="n">
-        <v>102.1335064516129</v>
+        <v>104.3648</v>
       </c>
       <c r="T8" t="n">
-        <v>72184.16129032258</v>
+        <v>73518.2</v>
       </c>
       <c r="U8" t="n">
-        <v>16533.59032258064</v>
+        <v>16954.42</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1526.926783870968</v>
+        <v>1379.234643333333</v>
       </c>
       <c r="B9" t="n">
-        <v>394.3451612903226</v>
+        <v>364.1366666666667</v>
       </c>
       <c r="C9" t="n">
-        <v>234.1483870967742</v>
+        <v>215.8333333333333</v>
       </c>
       <c r="D9" t="n">
-        <v>10.06666666666667</v>
+        <v>11</v>
       </c>
       <c r="E9" t="n">
-        <v>3.606451612903226</v>
+        <v>4.3</v>
       </c>
       <c r="F9" t="n">
-        <v>13.50333333333333</v>
+        <v>11.18</v>
       </c>
       <c r="G9" t="n">
-        <v>2325.921609677419</v>
+        <v>2075.974646666667</v>
       </c>
       <c r="H9" t="n">
-        <v>34.40322580645161</v>
+        <v>34.4</v>
       </c>
       <c r="I9" t="n">
-        <v>97.23870967741935</v>
+        <v>93.45333333333333</v>
       </c>
       <c r="J9" t="n">
-        <v>9.9055614</v>
+        <v>9.908494076923077</v>
       </c>
       <c r="K9" t="n">
-        <v>61.12333333333333</v>
+        <v>46.02</v>
       </c>
       <c r="L9" t="n">
-        <v>255.1342903225807</v>
+        <v>244.2403333333333</v>
       </c>
       <c r="M9" t="n">
-        <v>207.6672903225807</v>
+        <v>193.4973</v>
       </c>
       <c r="N9" t="n">
-        <v>2.419677419354838</v>
+        <v>1.146333333333333</v>
       </c>
       <c r="O9" t="n">
-        <v>0.04333333333333333</v>
+        <v>1.28</v>
       </c>
       <c r="P9" t="n">
         <v>0</v>
       </c>
       <c r="Q9" t="n">
-        <v>99.57553045249306</v>
+        <v>100.024757682087</v>
       </c>
       <c r="R9" t="n">
-        <v>127.6161290322581</v>
+        <v>121.4003333333333</v>
       </c>
       <c r="S9" t="n">
-        <v>102.3992903225806</v>
+        <v>100.1475666666667</v>
       </c>
       <c r="T9" t="n">
-        <v>67056.6129032258</v>
+        <v>61363.8</v>
       </c>
       <c r="U9" t="n">
-        <v>14326.56129032258</v>
+        <v>13197.58333333333</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1726.708025806452</v>
+        <v>1620.456493333333</v>
       </c>
       <c r="B10" t="n">
-        <v>580.5684838709677</v>
+        <v>536.7552000000001</v>
       </c>
       <c r="C10" t="n">
-        <v>405.3624193548387</v>
+        <v>417.4457</v>
       </c>
       <c r="D10" t="n">
-        <v>20.25</v>
+        <v>17.16</v>
       </c>
       <c r="E10" t="n">
-        <v>3.6</v>
+        <v>4.603333333333333</v>
       </c>
       <c r="F10" t="n">
-        <v>20.56</v>
+        <v>23.14</v>
       </c>
       <c r="G10" t="n">
-        <v>2560.214683870968</v>
+        <v>2417.547413333333</v>
       </c>
       <c r="H10" t="n">
-        <v>34.6</v>
+        <v>34.8</v>
       </c>
       <c r="I10" t="n">
-        <v>65.01290322580645</v>
+        <v>71.73666666666666</v>
       </c>
       <c r="J10" t="n">
-        <v>9.516867326086956</v>
+        <v>9.318259489130435</v>
       </c>
       <c r="K10" t="n">
-        <v>100.53</v>
+        <v>75.22</v>
       </c>
       <c r="L10" t="n">
-        <v>288.6321935483871</v>
+        <v>276.5108</v>
       </c>
       <c r="M10" t="n">
-        <v>300.6474516129032</v>
+        <v>273.6442</v>
       </c>
       <c r="N10" t="n">
-        <v>0.3258064516129032</v>
+        <v>0.08</v>
       </c>
       <c r="O10" t="n">
-        <v>1.8</v>
+        <v>1.48</v>
       </c>
       <c r="P10" t="n">
         <v>0</v>
       </c>
       <c r="Q10" t="n">
-        <v>99.72129721501773</v>
+        <v>100.3052101638742</v>
       </c>
       <c r="R10" t="n">
-        <v>133.7270967741935</v>
+        <v>129.8516666666667</v>
       </c>
       <c r="S10" t="n">
-        <v>104.4967935483871</v>
+        <v>101.3098533333333</v>
       </c>
       <c r="T10" t="n">
-        <v>73106.67741935483</v>
+        <v>70587.53333333334</v>
       </c>
       <c r="U10" t="n">
-        <v>16920.90967741936</v>
+        <v>16302.14666666667</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1575.50846</v>
+        <v>1554.142806451613</v>
       </c>
       <c r="B11" t="n">
-        <v>363.19</v>
+        <v>338.4935483870968</v>
       </c>
       <c r="C11" t="n">
-        <v>206.5966666666667</v>
+        <v>204.8903225806451</v>
       </c>
       <c r="D11" t="n">
-        <v>15.37</v>
+        <v>29.19</v>
       </c>
       <c r="E11" t="n">
-        <v>3.596666666666667</v>
+        <v>14.36774193548387</v>
       </c>
       <c r="F11" t="n">
-        <v>16.24</v>
+        <v>53.54</v>
       </c>
       <c r="G11" t="n">
-        <v>2369.373433333333</v>
+        <v>2906.205274193548</v>
       </c>
       <c r="H11" t="n">
-        <v>34.4</v>
+        <v>34.19677419354839</v>
       </c>
       <c r="I11" t="n">
-        <v>95.42333333333333</v>
+        <v>72.35806451612903</v>
       </c>
       <c r="J11" t="n">
-        <v>9.935092630434783</v>
+        <v>8.863368769230769</v>
       </c>
       <c r="K11" t="n">
-        <v>54.09</v>
+        <v>20.51</v>
       </c>
       <c r="L11" t="n">
-        <v>257.2813666666667</v>
+        <v>256.1608064516129</v>
       </c>
       <c r="M11" t="n">
-        <v>212.0108666666667</v>
+        <v>217.2059677419355</v>
       </c>
       <c r="N11" t="n">
-        <v>1.837</v>
+        <v>0.06935483870967751</v>
       </c>
       <c r="O11" t="n">
-        <v>-0.2</v>
+        <v>0.59</v>
       </c>
       <c r="P11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q11" t="n">
-        <v>99.22913027324101</v>
+        <v>93.34563685915909</v>
       </c>
       <c r="R11" t="n">
-        <v>129.0736666666667</v>
+        <v>115.9635483870968</v>
       </c>
       <c r="S11" t="n">
-        <v>101.8042166666667</v>
+        <v>85.37563225806451</v>
       </c>
       <c r="T11" t="n">
-        <v>65206.86666666667</v>
+        <v>55711.77419354839</v>
       </c>
       <c r="U11" t="n">
-        <v>14606.46</v>
+        <v>12077.94193548387</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1459.674851774193</v>
+        <v>1526.926783870968</v>
       </c>
       <c r="B12" t="n">
-        <v>406.9417204301075</v>
+        <v>394.3451612903226</v>
       </c>
       <c r="C12" t="n">
-        <v>233.862311827957</v>
+        <v>234.1483870967742</v>
       </c>
       <c r="D12" t="n">
-        <v>11.96</v>
+        <v>10.06666666666667</v>
       </c>
       <c r="E12" t="n">
-        <v>3.996666666666667</v>
+        <v>3.606451612903226</v>
       </c>
       <c r="F12" t="n">
-        <v>21.795</v>
+        <v>13.50333333333333</v>
       </c>
       <c r="G12" t="n">
-        <v>2161.494655860215</v>
+        <v>2325.921609677419</v>
       </c>
       <c r="H12" t="n">
-        <v>34.5</v>
+        <v>34.40322580645161</v>
       </c>
       <c r="I12" t="n">
-        <v>98.91247311827956</v>
+        <v>97.23870967741935</v>
       </c>
       <c r="J12" t="n">
-        <v>9.795628748168497</v>
+        <v>9.9055614</v>
       </c>
       <c r="K12" t="n">
-        <v>63.96</v>
+        <v>61.12333333333333</v>
       </c>
       <c r="L12" t="n">
-        <v>250.1292112903226</v>
+        <v>255.1342903225807</v>
       </c>
       <c r="M12" t="n">
-        <v>200.5677784946236</v>
+        <v>207.6672903225807</v>
       </c>
       <c r="N12" t="n">
-        <v>1.681456989247312</v>
+        <v>2.419677419354838</v>
       </c>
       <c r="O12" t="n">
-        <v>0.985</v>
+        <v>0.04333333333333333</v>
       </c>
       <c r="P12" t="n">
         <v>0</v>
       </c>
       <c r="Q12" t="n">
-        <v>100.6920865385476</v>
+        <v>99.57553045249306</v>
       </c>
       <c r="R12" t="n">
-        <v>124.0734677419355</v>
+        <v>127.6161290322581</v>
       </c>
       <c r="S12" t="n">
-        <v>103.3620803763441</v>
+        <v>102.3992903225806</v>
       </c>
       <c r="T12" t="n">
-        <v>65399.39462365591</v>
+        <v>67056.6129032258</v>
       </c>
       <c r="U12" t="n">
-        <v>13806.2676344086</v>
+        <v>14326.56129032258</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1524.761677419355</v>
+        <v>1575.50846</v>
       </c>
       <c r="B13" t="n">
-        <v>458.1193548387097</v>
+        <v>363.19</v>
       </c>
       <c r="C13" t="n">
-        <v>250.1516129032258</v>
+        <v>206.5966666666667</v>
       </c>
       <c r="D13" t="n">
-        <v>20.79</v>
+        <v>15.37</v>
       </c>
       <c r="E13" t="n">
-        <v>6.409677419354839</v>
+        <v>3.596666666666667</v>
       </c>
       <c r="F13" t="n">
-        <v>22.75</v>
+        <v>16.24</v>
       </c>
       <c r="G13" t="n">
-        <v>2569.302306451613</v>
+        <v>2369.373433333333</v>
       </c>
       <c r="H13" t="n">
-        <v>34.99032258064516</v>
+        <v>34.4</v>
       </c>
       <c r="I13" t="n">
-        <v>79.05483870967743</v>
+        <v>95.42333333333333</v>
       </c>
       <c r="J13" t="n">
-        <v>8.395245293478261</v>
+        <v>9.935092630434783</v>
       </c>
       <c r="K13" t="n">
-        <v>48.35</v>
+        <v>54.09</v>
       </c>
       <c r="L13" t="n">
-        <v>262.1794838709677</v>
+        <v>257.2813666666667</v>
       </c>
       <c r="M13" t="n">
-        <v>236.4399032258065</v>
+        <v>212.0108666666667</v>
       </c>
       <c r="N13" t="n">
-        <v>0.09</v>
+        <v>1.837</v>
       </c>
       <c r="O13" t="n">
-        <v>0.84</v>
+        <v>-0.2</v>
       </c>
       <c r="P13" t="n">
         <v>0</v>
       </c>
       <c r="Q13" t="n">
-        <v>99.79939459335134</v>
+        <v>99.22913027324101</v>
       </c>
       <c r="R13" t="n">
-        <v>124.2593548387097</v>
+        <v>129.0736666666667</v>
       </c>
       <c r="S13" t="n">
-        <v>99.22816129032257</v>
+        <v>101.8042166666667</v>
       </c>
       <c r="T13" t="n">
-        <v>64724</v>
+        <v>65206.86666666667</v>
       </c>
       <c r="U13" t="n">
-        <v>14842.79032258064</v>
+        <v>14606.46</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1530.413548387097</v>
+        <v>1407.679989390681</v>
       </c>
       <c r="B14" t="n">
-        <v>504.5</v>
+        <v>398.6220071684588</v>
       </c>
       <c r="C14" t="n">
-        <v>320.3612903225807</v>
+        <v>211.6576344086021</v>
       </c>
       <c r="D14" t="n">
-        <v>17.07</v>
+        <v>11.75333333333333</v>
       </c>
       <c r="E14" t="n">
-        <v>6</v>
+        <v>4.204444444444444</v>
       </c>
       <c r="F14" t="n">
-        <v>19.4</v>
+        <v>9.49</v>
       </c>
       <c r="G14" t="n">
-        <v>2552.336158064516</v>
+        <v>2111.770228530466</v>
       </c>
       <c r="H14" t="n">
-        <v>34.9</v>
+        <v>34.39663082437276</v>
       </c>
       <c r="I14" t="n">
-        <v>88.19032258064516</v>
+        <v>100.4274551971326</v>
       </c>
       <c r="J14" t="n">
-        <v>9.101889566666667</v>
+        <v>9.913020010869564</v>
       </c>
       <c r="K14" t="n">
-        <v>59.19</v>
+        <v>51.31</v>
       </c>
       <c r="L14" t="n">
-        <v>266.6721935483871</v>
+        <v>246.6245863799283</v>
       </c>
       <c r="M14" t="n">
-        <v>249.7142580645161</v>
+        <v>195.0992143369176</v>
       </c>
       <c r="N14" t="n">
-        <v>0.07000000000000001</v>
+        <v>1.15010752688172</v>
       </c>
       <c r="O14" t="n">
-        <v>1.71</v>
+        <v>1.29</v>
       </c>
       <c r="P14" t="n">
         <v>0</v>
       </c>
       <c r="Q14" t="n">
-        <v>100.5973786748587</v>
+        <v>100.2700716578218</v>
       </c>
       <c r="R14" t="n">
-        <v>125.9677419354839</v>
+        <v>122.2105663082437</v>
       </c>
       <c r="S14" t="n">
-        <v>99.01935806451614</v>
+        <v>100.9862233691756</v>
       </c>
       <c r="T14" t="n">
-        <v>67888.25806451614</v>
+        <v>63953.99569892474</v>
       </c>
       <c r="U14" t="n">
-        <v>15613.54516129032</v>
+        <v>13394.56494623656</v>
       </c>
     </row>
     <row r="15">
@@ -3030,457 +3189,457 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1759.5398</v>
+        <v>1459.674851774193</v>
       </c>
       <c r="B16" t="n">
-        <v>542.649</v>
+        <v>406.9417204301075</v>
       </c>
       <c r="C16" t="n">
-        <v>412.865</v>
+        <v>233.862311827957</v>
       </c>
       <c r="D16" t="n">
-        <v>19.61</v>
+        <v>11.96</v>
       </c>
       <c r="E16" t="n">
-        <v>3.6</v>
+        <v>3.996666666666667</v>
       </c>
       <c r="F16" t="n">
-        <v>28.71</v>
+        <v>21.795</v>
       </c>
       <c r="G16" t="n">
-        <v>2661.893</v>
+        <v>2161.494655860215</v>
       </c>
       <c r="H16" t="n">
         <v>34.5</v>
       </c>
       <c r="I16" t="n">
-        <v>58.85333333333333</v>
+        <v>98.91247311827956</v>
       </c>
       <c r="J16" t="n">
-        <v>9.516867326086956</v>
+        <v>9.795628748168497</v>
       </c>
       <c r="K16" t="n">
-        <v>107.76</v>
+        <v>63.96</v>
       </c>
       <c r="L16" t="n">
-        <v>295.328</v>
+        <v>250.1292112903226</v>
       </c>
       <c r="M16" t="n">
-        <v>300.845</v>
+        <v>200.5677784946236</v>
       </c>
       <c r="N16" t="n">
-        <v>1.21</v>
+        <v>1.681456989247312</v>
       </c>
       <c r="O16" t="n">
-        <v>1.26</v>
+        <v>0.985</v>
       </c>
       <c r="P16" t="n">
         <v>0</v>
       </c>
       <c r="Q16" t="n">
-        <v>99.4414473129178</v>
+        <v>100.6920865385476</v>
       </c>
       <c r="R16" t="n">
-        <v>134.1606666666667</v>
+        <v>124.0734677419355</v>
       </c>
       <c r="S16" t="n">
-        <v>104.3648</v>
+        <v>103.3620803763441</v>
       </c>
       <c r="T16" t="n">
-        <v>73518.2</v>
+        <v>65399.39462365591</v>
       </c>
       <c r="U16" t="n">
-        <v>16954.42</v>
+        <v>13806.2676344086</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1554.142806451613</v>
+        <v>1596.682522580645</v>
       </c>
       <c r="B17" t="n">
-        <v>338.4935483870968</v>
+        <v>376.5483870967742</v>
       </c>
       <c r="C17" t="n">
-        <v>204.8903225806451</v>
+        <v>211.9451612903226</v>
       </c>
       <c r="D17" t="n">
-        <v>29.19</v>
+        <v>12.63</v>
       </c>
       <c r="E17" t="n">
-        <v>14.36774193548387</v>
+        <v>3.503225806451613</v>
       </c>
       <c r="F17" t="n">
-        <v>53.54</v>
+        <v>13.78</v>
       </c>
       <c r="G17" t="n">
-        <v>2906.205274193548</v>
+        <v>2353.635316129032</v>
       </c>
       <c r="H17" t="n">
-        <v>34.19677419354839</v>
+        <v>34.3</v>
       </c>
       <c r="I17" t="n">
-        <v>72.35806451612903</v>
+        <v>99.78387096774193</v>
       </c>
       <c r="J17" t="n">
-        <v>8.863368769230769</v>
+        <v>9.855037173913043</v>
       </c>
       <c r="K17" t="n">
-        <v>20.51</v>
+        <v>61.14</v>
       </c>
       <c r="L17" t="n">
-        <v>256.1608064516129</v>
+        <v>258.6684838709677</v>
       </c>
       <c r="M17" t="n">
-        <v>217.2059677419355</v>
+        <v>212.4300967741935</v>
       </c>
       <c r="N17" t="n">
-        <v>0.06935483870967751</v>
+        <v>1.55</v>
       </c>
       <c r="O17" t="n">
-        <v>0.59</v>
+        <v>0.37</v>
       </c>
       <c r="P17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q17" t="n">
-        <v>93.34563685915909</v>
+        <v>99.17224194271503</v>
       </c>
       <c r="R17" t="n">
-        <v>115.9635483870968</v>
+        <v>130.0467741935484</v>
       </c>
       <c r="S17" t="n">
-        <v>85.37563225806451</v>
+        <v>101.3178451612903</v>
       </c>
       <c r="T17" t="n">
-        <v>55711.77419354839</v>
+        <v>62319.03225806452</v>
       </c>
       <c r="U17" t="n">
-        <v>12077.94193548387</v>
+        <v>14767.20322580645</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1379.234643333333</v>
+        <v>1726.708025806452</v>
       </c>
       <c r="B18" t="n">
-        <v>364.1366666666667</v>
+        <v>580.5684838709677</v>
       </c>
       <c r="C18" t="n">
-        <v>215.8333333333333</v>
+        <v>405.3624193548387</v>
       </c>
       <c r="D18" t="n">
-        <v>11</v>
+        <v>20.25</v>
       </c>
       <c r="E18" t="n">
-        <v>4.3</v>
+        <v>3.6</v>
       </c>
       <c r="F18" t="n">
-        <v>11.18</v>
+        <v>20.56</v>
       </c>
       <c r="G18" t="n">
-        <v>2075.974646666667</v>
+        <v>2560.214683870968</v>
       </c>
       <c r="H18" t="n">
-        <v>34.4</v>
+        <v>34.6</v>
       </c>
       <c r="I18" t="n">
-        <v>93.45333333333333</v>
+        <v>65.01290322580645</v>
       </c>
       <c r="J18" t="n">
-        <v>9.908494076923077</v>
+        <v>9.516867326086956</v>
       </c>
       <c r="K18" t="n">
-        <v>46.02</v>
+        <v>100.53</v>
       </c>
       <c r="L18" t="n">
-        <v>244.2403333333333</v>
+        <v>288.6321935483871</v>
       </c>
       <c r="M18" t="n">
-        <v>193.4973</v>
+        <v>300.6474516129032</v>
       </c>
       <c r="N18" t="n">
-        <v>1.146333333333333</v>
+        <v>0.3258064516129032</v>
       </c>
       <c r="O18" t="n">
-        <v>1.28</v>
+        <v>1.8</v>
       </c>
       <c r="P18" t="n">
         <v>0</v>
       </c>
       <c r="Q18" t="n">
-        <v>100.024757682087</v>
+        <v>99.72129721501773</v>
       </c>
       <c r="R18" t="n">
-        <v>121.4003333333333</v>
+        <v>133.7270967741935</v>
       </c>
       <c r="S18" t="n">
-        <v>100.1475666666667</v>
+        <v>104.4967935483871</v>
       </c>
       <c r="T18" t="n">
-        <v>61363.8</v>
+        <v>73106.67741935483</v>
       </c>
       <c r="U18" t="n">
-        <v>13197.58333333333</v>
+        <v>16920.90967741936</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1596.682522580645</v>
+        <v>1524.761677419355</v>
       </c>
       <c r="B19" t="n">
-        <v>376.5483870967742</v>
+        <v>458.1193548387097</v>
       </c>
       <c r="C19" t="n">
-        <v>211.9451612903226</v>
+        <v>250.1516129032258</v>
       </c>
       <c r="D19" t="n">
-        <v>12.63</v>
+        <v>20.79</v>
       </c>
       <c r="E19" t="n">
-        <v>3.503225806451613</v>
+        <v>6.409677419354839</v>
       </c>
       <c r="F19" t="n">
-        <v>13.78</v>
+        <v>22.75</v>
       </c>
       <c r="G19" t="n">
-        <v>2353.635316129032</v>
+        <v>2569.302306451613</v>
       </c>
       <c r="H19" t="n">
-        <v>34.3</v>
+        <v>34.99032258064516</v>
       </c>
       <c r="I19" t="n">
-        <v>99.78387096774193</v>
+        <v>79.05483870967743</v>
       </c>
       <c r="J19" t="n">
-        <v>9.855037173913043</v>
+        <v>8.395245293478261</v>
       </c>
       <c r="K19" t="n">
-        <v>61.14</v>
+        <v>48.35</v>
       </c>
       <c r="L19" t="n">
-        <v>258.6684838709677</v>
+        <v>262.1794838709677</v>
       </c>
       <c r="M19" t="n">
-        <v>212.4300967741935</v>
+        <v>236.4399032258065</v>
       </c>
       <c r="N19" t="n">
-        <v>1.55</v>
+        <v>0.09</v>
       </c>
       <c r="O19" t="n">
-        <v>0.37</v>
+        <v>0.84</v>
       </c>
       <c r="P19" t="n">
         <v>0</v>
       </c>
       <c r="Q19" t="n">
-        <v>99.17224194271503</v>
+        <v>99.79939459335134</v>
       </c>
       <c r="R19" t="n">
-        <v>130.0467741935484</v>
+        <v>124.2593548387097</v>
       </c>
       <c r="S19" t="n">
-        <v>101.3178451612903</v>
+        <v>99.22816129032257</v>
       </c>
       <c r="T19" t="n">
-        <v>62319.03225806452</v>
+        <v>64724</v>
       </c>
       <c r="U19" t="n">
-        <v>14767.20322580645</v>
+        <v>14842.79032258064</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1620.456493333333</v>
+        <v>1433.161535483871</v>
       </c>
       <c r="B20" t="n">
-        <v>536.7552000000001</v>
+        <v>410.1193548387097</v>
       </c>
       <c r="C20" t="n">
-        <v>417.4457</v>
+        <v>217.4451612903226</v>
       </c>
       <c r="D20" t="n">
-        <v>17.16</v>
+        <v>11.46</v>
       </c>
       <c r="E20" t="n">
-        <v>4.603333333333333</v>
+        <v>4.006451612903225</v>
       </c>
       <c r="F20" t="n">
-        <v>23.14</v>
+        <v>10.405</v>
       </c>
       <c r="G20" t="n">
-        <v>2417.547413333333</v>
+        <v>2107.725608064516</v>
       </c>
       <c r="H20" t="n">
-        <v>34.8</v>
+        <v>34.40645161290323</v>
       </c>
       <c r="I20" t="n">
-        <v>71.73666666666666</v>
+        <v>95.7741935483871</v>
       </c>
       <c r="J20" t="n">
-        <v>9.318259489130435</v>
+        <v>9.846498242149758</v>
       </c>
       <c r="K20" t="n">
-        <v>75.22</v>
+        <v>60.415</v>
       </c>
       <c r="L20" t="n">
-        <v>276.5108</v>
+        <v>248.7088387096774</v>
       </c>
       <c r="M20" t="n">
-        <v>273.6442</v>
+        <v>196.1336774193548</v>
       </c>
       <c r="N20" t="n">
-        <v>0.08</v>
+        <v>1.404838709677419</v>
       </c>
       <c r="O20" t="n">
-        <v>1.48</v>
+        <v>1.015</v>
       </c>
       <c r="P20" t="n">
         <v>0</v>
       </c>
       <c r="Q20" t="n">
-        <v>100.3052101638742</v>
+        <v>100.5199462359304</v>
       </c>
       <c r="R20" t="n">
-        <v>129.8516666666667</v>
+        <v>123.0925806451613</v>
       </c>
       <c r="S20" t="n">
-        <v>101.3098533333333</v>
+        <v>101.3529064516129</v>
       </c>
       <c r="T20" t="n">
-        <v>70587.53333333334</v>
+        <v>63835.80645161291</v>
       </c>
       <c r="U20" t="n">
-        <v>16302.14666666667</v>
+        <v>13619.81290322581</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1471.535181218638</v>
+        <v>1530.413548387097</v>
       </c>
       <c r="B21" t="n">
-        <v>398.0820788530465</v>
+        <v>504.5</v>
       </c>
       <c r="C21" t="n">
-        <v>244.225376344086</v>
+        <v>320.3612903225807</v>
       </c>
       <c r="D21" t="n">
-        <v>11.08333333333333</v>
+        <v>17.07</v>
       </c>
       <c r="E21" t="n">
-        <v>3.808888888888889</v>
+        <v>6</v>
       </c>
       <c r="F21" t="n">
-        <v>15.92666666666667</v>
+        <v>19.4</v>
       </c>
       <c r="G21" t="n">
-        <v>2200.957183655914</v>
+        <v>2552.336158064516</v>
       </c>
       <c r="H21" t="n">
-        <v>34.5</v>
+        <v>34.9</v>
       </c>
       <c r="I21" t="n">
-        <v>97.89505376344086</v>
+        <v>88.19032258064516</v>
       </c>
       <c r="J21" t="n">
-        <v>9.797889828555501</v>
+        <v>9.101889566666667</v>
       </c>
       <c r="K21" t="n">
-        <v>74.05</v>
+        <v>59.19</v>
       </c>
       <c r="L21" t="n">
-        <v>251.3184695340502</v>
+        <v>266.6721935483871</v>
       </c>
       <c r="M21" t="n">
-        <v>204.9377089605735</v>
+        <v>249.7142580645161</v>
       </c>
       <c r="N21" t="n">
-        <v>1.906</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="O21" t="n">
-        <v>0.91</v>
+        <v>1.71</v>
       </c>
       <c r="P21" t="n">
         <v>0</v>
       </c>
       <c r="Q21" t="n">
-        <v>100.6185806839007</v>
+        <v>100.5973786748587</v>
       </c>
       <c r="R21" t="n">
-        <v>125.0281146953405</v>
+        <v>125.9677419354839</v>
       </c>
       <c r="S21" t="n">
-        <v>103.4573125448029</v>
+        <v>99.01935806451614</v>
       </c>
       <c r="T21" t="n">
-        <v>68361.42939068101</v>
+        <v>67888.25806451614</v>
       </c>
       <c r="U21" t="n">
-        <v>13960.94917562724</v>
+        <v>15613.54516129032</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1580.510146666667</v>
+        <v>1488.268166666667</v>
       </c>
       <c r="B22" t="n">
-        <v>542.1844333333333</v>
+        <v>376.0766666666667</v>
       </c>
       <c r="C22" t="n">
-        <v>381.8903</v>
+        <v>244.12</v>
       </c>
       <c r="D22" t="n">
-        <v>15.97</v>
+        <v>10.93333333333333</v>
       </c>
       <c r="E22" t="n">
-        <v>5.416666666666667</v>
+        <v>3.796666666666666</v>
       </c>
       <c r="F22" t="n">
-        <v>15.83</v>
+        <v>12.04</v>
       </c>
       <c r="G22" t="n">
-        <v>2448.47103</v>
+        <v>2247.25593</v>
       </c>
       <c r="H22" t="n">
-        <v>34.8</v>
+        <v>34.5</v>
       </c>
       <c r="I22" t="n">
-        <v>81.34333333333333</v>
+        <v>98.64999999999999</v>
       </c>
       <c r="J22" t="n">
-        <v>9.20270443956044</v>
+        <v>9.811155195652175</v>
       </c>
       <c r="K22" t="n">
-        <v>73.52</v>
+        <v>74.63333333333334</v>
       </c>
       <c r="L22" t="n">
-        <v>272.1430333333333</v>
+        <v>252.8412333333333</v>
       </c>
       <c r="M22" t="n">
-        <v>265.4335</v>
+        <v>205.3912</v>
       </c>
       <c r="N22" t="n">
-        <v>0.09933333333333333</v>
+        <v>2.182</v>
       </c>
       <c r="O22" t="n">
-        <v>1.4</v>
+        <v>0.86</v>
       </c>
       <c r="P22" t="n">
         <v>0</v>
       </c>
       <c r="Q22" t="n">
-        <v>100.5441661244718</v>
+        <v>100.2896470386735</v>
       </c>
       <c r="R22" t="n">
-        <v>127.9216666666667</v>
+        <v>125.8326666666667</v>
       </c>
       <c r="S22" t="n">
-        <v>100.84973</v>
+        <v>104.0515633333333</v>
       </c>
       <c r="T22" t="n">
-        <v>68643.26666666666</v>
+        <v>67904.2</v>
       </c>
       <c r="U22" t="n">
-        <v>15814.47</v>
+        <v>14116.63666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added trending calculations and correlations comparing futures to sp500
</commit_message>
<xml_diff>
--- a/code/Screener/reports/2022-07-15_completed_fred_pvt.xlsx
+++ b/code/Screener/reports/2022-07-15_completed_fred_pvt.xlsx
@@ -986,6 +986,56 @@
     </pic>
     <clientData/>
   </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>1</col>
+      <colOff>0</colOff>
+      <row>595</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="10353675" cy="4838700"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="23" name="Image 23" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId23"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>1</col>
+      <colOff>0</colOff>
+      <row>622</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="10315575" cy="4838700"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="24" name="Image 24" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId24"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
 </wsDr>
 </file>
 
@@ -1278,7 +1328,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1531,6 +1581,142 @@
         <v>1</v>
       </c>
       <c r="V3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" t="n">
+        <v>1</v>
+      </c>
+      <c r="M4" t="n">
+        <v>1</v>
+      </c>
+      <c r="N4" t="n">
+        <v>1</v>
+      </c>
+      <c r="O4" t="n">
+        <v>1</v>
+      </c>
+      <c r="P4" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>1</v>
+      </c>
+      <c r="R4" t="n">
+        <v>1</v>
+      </c>
+      <c r="S4" t="n">
+        <v>1</v>
+      </c>
+      <c r="T4" t="n">
+        <v>1</v>
+      </c>
+      <c r="U4" t="n">
+        <v>1</v>
+      </c>
+      <c r="V4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N5" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" t="n">
+        <v>1</v>
+      </c>
+      <c r="P5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>1</v>
+      </c>
+      <c r="R5" t="n">
+        <v>1</v>
+      </c>
+      <c r="S5" t="n">
+        <v>1</v>
+      </c>
+      <c r="T5" t="n">
+        <v>1</v>
+      </c>
+      <c r="U5" t="n">
+        <v>1</v>
+      </c>
+      <c r="V5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1621,7 +1807,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1644,6 +1830,16 @@
     <row r="3">
       <c r="A3" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1657,7 +1853,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE3"/>
+  <dimension ref="A1:AO5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1821,6 +2017,56 @@
           <t>b</t>
         </is>
       </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>prior</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>remove</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>not_remove</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>best_to_follow</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>my_string</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>t_</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>right</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>index_</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -2042,6 +2288,254 @@
       </c>
       <c r="AE3" t="n">
         <v>0.9859267780170259</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>CONSUMER,WPUSI019011,WPU101,GVZCLS,UNRATE,VIXCLS,BUSLOANS,AWHAETP,UMCSENT,TDSP,DCOILWTICO,CPIAUCSL,CSUSHPINSA,FEDFUNDS,T10Y3M,USREC,USALOLITONOSTSAM,USPHCI,INDPRO,NEWORDER,PCE,</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2022-07-16 15:46:37</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>C:\Users\User\Documents\wiki\wiki\dev\python\Python-Stock\code\Screener\code</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>13</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2022-07-14</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>..\data\\interim\\Business Cycles-2.png</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>AWHAETP</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>9</v>
+      </c>
+      <c r="J4" t="n">
+        <v>25.0042277619534</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.2725588811642105</v>
+      </c>
+      <c r="L4" t="n">
+        <v>222.4253656575287</v>
+      </c>
+      <c r="M4" t="n">
+        <v>95.08377751526875</v>
+      </c>
+      <c r="N4" t="n">
+        <v>2</v>
+      </c>
+      <c r="O4" t="n">
+        <v>5</v>
+      </c>
+      <c r="P4" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>6</v>
+      </c>
+      <c r="R4" t="n">
+        <v>197.8430095399954</v>
+      </c>
+      <c r="S4" t="n">
+        <v>24.98327344733859</v>
+      </c>
+      <c r="T4" t="n">
+        <v>6.254103901426333e-10</v>
+      </c>
+      <c r="U4" t="n">
+        <v>2</v>
+      </c>
+      <c r="V4" t="n">
+        <v>8.212685127145461</v>
+      </c>
+      <c r="W4" t="n">
+        <v>2</v>
+      </c>
+      <c r="X4" t="n">
+        <v>6</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>20</v>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>PCE</t>
+        </is>
+      </c>
+      <c r="AB4" t="n">
+        <v>0.9859267780170259</v>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>CPIAUCSL</t>
+        </is>
+      </c>
+      <c r="AD4" t="n">
+        <v>0.9341681412934574</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>0.9859267780170259</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG4" t="inlineStr">
+        <is>
+          <t>CSUSHPINSA</t>
+        </is>
+      </c>
+      <c r="AH4" t="inlineStr">
+        <is>
+          <t>CPIAUCSL</t>
+        </is>
+      </c>
+      <c r="AI4" t="inlineStr">
+        <is>
+          <t>DCOILWTICO</t>
+        </is>
+      </c>
+      <c r="AJ4" t="inlineStr">
+        <is>
+          <t>AWHAETP UNRATE</t>
+        </is>
+      </c>
+      <c r="AK4" t="inlineStr">
+        <is>
+          <t>UNRATE AWHAETP</t>
+        </is>
+      </c>
+      <c r="AL4" t="n">
+        <v>209</v>
+      </c>
+      <c r="AM4" t="inlineStr">
+        <is>
+          <t>AWHAETP</t>
+        </is>
+      </c>
+      <c r="AN4" t="inlineStr">
+        <is>
+          <t>UNRATE</t>
+        </is>
+      </c>
+      <c r="AO4" t="inlineStr">
+        <is>
+          <t>CONSUMER CPIAUCSL</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>CONSUMER,WPUSI019011,WPU101,GVZCLS,UNRATE,VIXCLS,BUSLOANS,AWHAETP,UMCSENT,TDSP,DCOILWTICO,CPIAUCSL,CSUSHPINSA,FEDFUNDS,T10Y3M,USREC,USALOLITONOSTSAM,USPHCI,INDPRO,NEWORDER,PCE,</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2022-07-16 16:29:20</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>C:\Users\User\Documents\wiki\wiki\dev\python\Python-Stock\code\Screener\code</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>13</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2022-07-14</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>..\data\\interim\\Business Cycles-2.png</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>WPU101</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>9</v>
+      </c>
+      <c r="J5" t="n">
+        <v>25.0042277619534</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.2725588811642105</v>
+      </c>
+      <c r="L5" t="n">
+        <v>222.4253656575287</v>
+      </c>
+      <c r="M5" t="n">
+        <v>95.08377751526876</v>
+      </c>
+      <c r="N5" t="n">
+        <v>2</v>
+      </c>
+      <c r="O5" t="n">
+        <v>5</v>
+      </c>
+      <c r="P5" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>6</v>
+      </c>
+      <c r="R5" t="n">
+        <v>197.8430095399954</v>
+      </c>
+      <c r="S5" t="n">
+        <v>24.98327344733859</v>
+      </c>
+      <c r="T5" t="n">
+        <v>6.254103901426333e-10</v>
+      </c>
+      <c r="U5" t="n">
+        <v>2</v>
+      </c>
+      <c r="V5" t="n">
+        <v>7.128404922900172</v>
+      </c>
+      <c r="W5" t="n">
+        <v>2</v>
+      </c>
+      <c r="X5" t="n">
+        <v>6</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>20</v>
+      </c>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>PCE</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -2055,7 +2549,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2148,6 +2642,62 @@
       <c r="F3" t="inlineStr">
         <is>
           <t>2022-07-16 10:27:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>fred_data</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>EDA-fred</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>AnalyzeSP1500.ipynb</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2022-07-16 15:46:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>fred_data</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>EDA-fred</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>AnalyzeSP1500.ipynb</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2022-07-16 16:29:20</t>
         </is>
       </c>
     </row>
@@ -2279,977 +2829,977 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1518.70469</v>
+        <v>1433.161535483871</v>
       </c>
       <c r="B2" t="n">
-        <v>396.4766666666667</v>
+        <v>410.1193548387097</v>
       </c>
       <c r="C2" t="n">
-        <v>207.3266666666667</v>
+        <v>217.4451612903226</v>
       </c>
       <c r="D2" t="n">
-        <v>22.07</v>
+        <v>11.46</v>
       </c>
       <c r="E2" t="n">
-        <v>6.933333333333334</v>
+        <v>4.006451612903225</v>
       </c>
       <c r="F2" t="n">
-        <v>26.37</v>
+        <v>10.405</v>
       </c>
       <c r="G2" t="n">
-        <v>2698.391866666667</v>
+        <v>2107.725608064516</v>
       </c>
       <c r="H2" t="n">
-        <v>34.89666666666667</v>
+        <v>34.40645161290323</v>
       </c>
       <c r="I2" t="n">
-        <v>81.75333333333333</v>
+        <v>95.7741935483871</v>
       </c>
       <c r="J2" t="n">
-        <v>9.402214543478262</v>
+        <v>9.846498242149758</v>
       </c>
       <c r="K2" t="n">
-        <v>40.05</v>
+        <v>60.415</v>
       </c>
       <c r="L2" t="n">
-        <v>260.3466</v>
+        <v>248.7088387096774</v>
       </c>
       <c r="M2" t="n">
-        <v>229.7583333333334</v>
+        <v>196.1336774193548</v>
       </c>
       <c r="N2" t="n">
-        <v>0.09</v>
+        <v>1.404838709677419</v>
       </c>
       <c r="O2" t="n">
-        <v>0.59</v>
+        <v>1.015</v>
       </c>
       <c r="P2" t="n">
         <v>0</v>
       </c>
       <c r="Q2" t="n">
-        <v>98.79102009760062</v>
+        <v>100.5199462359304</v>
       </c>
       <c r="R2" t="n">
-        <v>122.8773333333333</v>
+        <v>123.0925806451613</v>
       </c>
       <c r="S2" t="n">
-        <v>96.79987</v>
+        <v>101.3529064516129</v>
       </c>
       <c r="T2" t="n">
-        <v>62779.6</v>
+        <v>63835.80645161291</v>
       </c>
       <c r="U2" t="n">
-        <v>14543.85666666667</v>
+        <v>13619.81290322581</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1518.463696666667</v>
+        <v>1459.674851774193</v>
       </c>
       <c r="B3" t="n">
-        <v>382.71</v>
+        <v>406.9417204301075</v>
       </c>
       <c r="C3" t="n">
-        <v>200.9866666666667</v>
+        <v>233.862311827957</v>
       </c>
       <c r="D3" t="n">
-        <v>19.65</v>
+        <v>11.96</v>
       </c>
       <c r="E3" t="n">
-        <v>10.22666666666667</v>
+        <v>3.996666666666667</v>
       </c>
       <c r="F3" t="n">
-        <v>30.43</v>
+        <v>21.795</v>
       </c>
       <c r="G3" t="n">
-        <v>2858.75815</v>
+        <v>2161.494655860215</v>
       </c>
       <c r="H3" t="n">
-        <v>34.6</v>
+        <v>34.5</v>
       </c>
       <c r="I3" t="n">
-        <v>72.68666666666667</v>
+        <v>98.91247311827956</v>
       </c>
       <c r="J3" t="n">
-        <v>9.193901098901099</v>
+        <v>9.795628748168497</v>
       </c>
       <c r="K3" t="n">
-        <v>39.27</v>
+        <v>63.96</v>
       </c>
       <c r="L3" t="n">
-        <v>258.4988</v>
+        <v>250.1292112903226</v>
       </c>
       <c r="M3" t="n">
-        <v>221.5394333333333</v>
+        <v>200.5677784946236</v>
       </c>
       <c r="N3" t="n">
-        <v>0.08966666666666666</v>
+        <v>1.681456989247312</v>
       </c>
       <c r="O3" t="n">
-        <v>0.5</v>
+        <v>0.985</v>
       </c>
       <c r="P3" t="n">
         <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>97.62538150086982</v>
+        <v>100.6920865385476</v>
       </c>
       <c r="R3" t="n">
-        <v>119.739</v>
+        <v>124.0734677419355</v>
       </c>
       <c r="S3" t="n">
-        <v>95.12751333333333</v>
+        <v>103.3620803763441</v>
       </c>
       <c r="T3" t="n">
-        <v>60043.43333333333</v>
+        <v>65399.39462365591</v>
       </c>
       <c r="U3" t="n">
-        <v>14121.20333333333</v>
+        <v>13806.2676344086</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1580.510146666667</v>
+        <v>1665.835980645161</v>
       </c>
       <c r="B4" t="n">
-        <v>542.1844333333333</v>
+        <v>549.6875806451612</v>
       </c>
       <c r="C4" t="n">
-        <v>381.8903</v>
+        <v>423.7149032258064</v>
       </c>
       <c r="D4" t="n">
-        <v>15.97</v>
+        <v>14.61</v>
       </c>
       <c r="E4" t="n">
-        <v>5.416666666666667</v>
+        <v>3.996774193548387</v>
       </c>
       <c r="F4" t="n">
-        <v>15.83</v>
+        <v>17.22</v>
       </c>
       <c r="G4" t="n">
-        <v>2448.47103</v>
+        <v>2487.060125806452</v>
       </c>
       <c r="H4" t="n">
-        <v>34.8</v>
+        <v>34.60645161290323</v>
       </c>
       <c r="I4" t="n">
-        <v>81.34333333333333</v>
+        <v>67.30967741935484</v>
       </c>
       <c r="J4" t="n">
-        <v>9.20270443956044</v>
+        <v>9.516867326086956</v>
       </c>
       <c r="K4" t="n">
-        <v>73.52</v>
+        <v>75.33</v>
       </c>
       <c r="L4" t="n">
-        <v>272.1430333333333</v>
+        <v>281.8747096774193</v>
       </c>
       <c r="M4" t="n">
-        <v>265.4335</v>
+        <v>281.9601290322581</v>
       </c>
       <c r="N4" t="n">
-        <v>0.09933333333333333</v>
+        <v>0.08</v>
       </c>
       <c r="O4" t="n">
-        <v>1.4</v>
+        <v>1.46</v>
       </c>
       <c r="P4" t="n">
         <v>0</v>
       </c>
       <c r="Q4" t="n">
-        <v>100.5441661244718</v>
+        <v>100.0793983529852</v>
       </c>
       <c r="R4" t="n">
-        <v>127.9216666666667</v>
+        <v>131.7567741935484</v>
       </c>
       <c r="S4" t="n">
-        <v>100.84973</v>
+        <v>102.1335064516129</v>
       </c>
       <c r="T4" t="n">
-        <v>68643.26666666666</v>
+        <v>72184.16129032258</v>
       </c>
       <c r="U4" t="n">
-        <v>15814.47</v>
+        <v>16533.59032258064</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1471.535181218638</v>
+        <v>1407.679989390681</v>
       </c>
       <c r="B5" t="n">
-        <v>398.0820788530465</v>
+        <v>398.6220071684588</v>
       </c>
       <c r="C5" t="n">
-        <v>244.225376344086</v>
+        <v>211.6576344086021</v>
       </c>
       <c r="D5" t="n">
-        <v>11.08333333333333</v>
+        <v>11.75333333333333</v>
       </c>
       <c r="E5" t="n">
-        <v>3.808888888888889</v>
+        <v>4.204444444444444</v>
       </c>
       <c r="F5" t="n">
-        <v>15.92666666666667</v>
+        <v>9.49</v>
       </c>
       <c r="G5" t="n">
-        <v>2200.957183655914</v>
+        <v>2111.770228530466</v>
       </c>
       <c r="H5" t="n">
-        <v>34.5</v>
+        <v>34.39663082437276</v>
       </c>
       <c r="I5" t="n">
-        <v>97.89505376344086</v>
+        <v>100.4274551971326</v>
       </c>
       <c r="J5" t="n">
-        <v>9.797889828555501</v>
+        <v>9.913020010869564</v>
       </c>
       <c r="K5" t="n">
-        <v>74.05</v>
+        <v>51.31</v>
       </c>
       <c r="L5" t="n">
-        <v>251.3184695340502</v>
+        <v>246.6245863799283</v>
       </c>
       <c r="M5" t="n">
-        <v>204.9377089605735</v>
+        <v>195.0992143369176</v>
       </c>
       <c r="N5" t="n">
-        <v>1.906</v>
+        <v>1.15010752688172</v>
       </c>
       <c r="O5" t="n">
-        <v>0.91</v>
+        <v>1.29</v>
       </c>
       <c r="P5" t="n">
         <v>0</v>
       </c>
       <c r="Q5" t="n">
-        <v>100.6185806839007</v>
+        <v>100.2700716578218</v>
       </c>
       <c r="R5" t="n">
-        <v>125.0281146953405</v>
+        <v>122.2105663082437</v>
       </c>
       <c r="S5" t="n">
-        <v>103.4573125448029</v>
+        <v>100.9862233691756</v>
       </c>
       <c r="T5" t="n">
-        <v>68361.42939068101</v>
+        <v>63953.99569892474</v>
       </c>
       <c r="U5" t="n">
-        <v>13960.94917562724</v>
+        <v>13394.56494623656</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1665.835980645161</v>
+        <v>1554.142806451613</v>
       </c>
       <c r="B6" t="n">
-        <v>549.6875806451612</v>
+        <v>338.4935483870968</v>
       </c>
       <c r="C6" t="n">
-        <v>423.7149032258064</v>
+        <v>204.8903225806451</v>
       </c>
       <c r="D6" t="n">
-        <v>14.61</v>
+        <v>29.19</v>
       </c>
       <c r="E6" t="n">
-        <v>3.996774193548387</v>
+        <v>14.36774193548387</v>
       </c>
       <c r="F6" t="n">
-        <v>17.22</v>
+        <v>53.54</v>
       </c>
       <c r="G6" t="n">
-        <v>2487.060125806452</v>
+        <v>2906.205274193548</v>
       </c>
       <c r="H6" t="n">
-        <v>34.60645161290323</v>
+        <v>34.19677419354839</v>
       </c>
       <c r="I6" t="n">
-        <v>67.30967741935484</v>
+        <v>72.35806451612903</v>
       </c>
       <c r="J6" t="n">
-        <v>9.516867326086956</v>
+        <v>8.863368769230769</v>
       </c>
       <c r="K6" t="n">
-        <v>75.33</v>
+        <v>20.51</v>
       </c>
       <c r="L6" t="n">
-        <v>281.8747096774193</v>
+        <v>256.1608064516129</v>
       </c>
       <c r="M6" t="n">
-        <v>281.9601290322581</v>
+        <v>217.2059677419355</v>
       </c>
       <c r="N6" t="n">
-        <v>0.08</v>
+        <v>0.06935483870967751</v>
       </c>
       <c r="O6" t="n">
-        <v>1.46</v>
+        <v>0.59</v>
       </c>
       <c r="P6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q6" t="n">
-        <v>100.0793983529852</v>
+        <v>93.34563685915909</v>
       </c>
       <c r="R6" t="n">
-        <v>131.7567741935484</v>
+        <v>115.9635483870968</v>
       </c>
       <c r="S6" t="n">
-        <v>102.1335064516129</v>
+        <v>85.37563225806451</v>
       </c>
       <c r="T6" t="n">
-        <v>72184.16129032258</v>
+        <v>55711.77419354839</v>
       </c>
       <c r="U6" t="n">
-        <v>16533.59032258064</v>
+        <v>12077.94193548387</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1549.487913333333</v>
+        <v>1488.268166666667</v>
       </c>
       <c r="B7" t="n">
-        <v>373.61</v>
+        <v>376.0766666666667</v>
       </c>
       <c r="C7" t="n">
-        <v>217.0866666666667</v>
+        <v>244.12</v>
       </c>
       <c r="D7" t="n">
-        <v>14.71666666666667</v>
+        <v>10.93333333333333</v>
       </c>
       <c r="E7" t="n">
-        <v>3.696666666666667</v>
+        <v>3.796666666666666</v>
       </c>
       <c r="F7" t="n">
-        <v>14.4</v>
+        <v>12.04</v>
       </c>
       <c r="G7" t="n">
-        <v>2343.950213333334</v>
+        <v>2247.25593</v>
       </c>
       <c r="H7" t="n">
-        <v>34.4</v>
+        <v>34.5</v>
       </c>
       <c r="I7" t="n">
-        <v>98.39333333333335</v>
+        <v>98.64999999999999</v>
       </c>
       <c r="J7" t="n">
-        <v>9.939332252747253</v>
+        <v>9.811155195652175</v>
       </c>
       <c r="K7" t="n">
-        <v>58.67333333333333</v>
+        <v>74.63333333333334</v>
       </c>
       <c r="L7" t="n">
-        <v>255.8820333333333</v>
+        <v>252.8412333333333</v>
       </c>
       <c r="M7" t="n">
-        <v>211.3559333333333</v>
+        <v>205.3912</v>
       </c>
       <c r="N7" t="n">
-        <v>2.399333333333333</v>
+        <v>2.182</v>
       </c>
       <c r="O7" t="n">
-        <v>-0.16</v>
+        <v>0.86</v>
       </c>
       <c r="P7" t="n">
         <v>0</v>
       </c>
       <c r="Q7" t="n">
-        <v>99.32935104420365</v>
+        <v>100.2896470386735</v>
       </c>
       <c r="R7" t="n">
-        <v>128.3126666666667</v>
+        <v>125.8326666666667</v>
       </c>
       <c r="S7" t="n">
-        <v>102.2142533333333</v>
+        <v>104.0515633333333</v>
       </c>
       <c r="T7" t="n">
-        <v>65884.36666666667</v>
+        <v>67904.2</v>
       </c>
       <c r="U7" t="n">
-        <v>14485.34333333333</v>
+        <v>14116.63666666667</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1759.5398</v>
+        <v>1549.487913333333</v>
       </c>
       <c r="B8" t="n">
-        <v>542.649</v>
+        <v>373.61</v>
       </c>
       <c r="C8" t="n">
-        <v>412.865</v>
+        <v>217.0866666666667</v>
       </c>
       <c r="D8" t="n">
-        <v>19.61</v>
+        <v>14.71666666666667</v>
       </c>
       <c r="E8" t="n">
-        <v>3.6</v>
+        <v>3.696666666666667</v>
       </c>
       <c r="F8" t="n">
-        <v>28.71</v>
+        <v>14.4</v>
       </c>
       <c r="G8" t="n">
-        <v>2661.893</v>
+        <v>2343.950213333334</v>
       </c>
       <c r="H8" t="n">
-        <v>34.5</v>
+        <v>34.4</v>
       </c>
       <c r="I8" t="n">
-        <v>58.85333333333333</v>
+        <v>98.39333333333335</v>
       </c>
       <c r="J8" t="n">
-        <v>9.516867326086956</v>
+        <v>9.939332252747253</v>
       </c>
       <c r="K8" t="n">
-        <v>107.76</v>
+        <v>58.67333333333333</v>
       </c>
       <c r="L8" t="n">
-        <v>295.328</v>
+        <v>255.8820333333333</v>
       </c>
       <c r="M8" t="n">
-        <v>300.845</v>
+        <v>211.3559333333333</v>
       </c>
       <c r="N8" t="n">
-        <v>1.21</v>
+        <v>2.399333333333333</v>
       </c>
       <c r="O8" t="n">
-        <v>1.26</v>
+        <v>-0.16</v>
       </c>
       <c r="P8" t="n">
         <v>0</v>
       </c>
       <c r="Q8" t="n">
-        <v>99.4414473129178</v>
+        <v>99.32935104420365</v>
       </c>
       <c r="R8" t="n">
-        <v>134.1606666666667</v>
+        <v>128.3126666666667</v>
       </c>
       <c r="S8" t="n">
-        <v>104.3648</v>
+        <v>102.2142533333333</v>
       </c>
       <c r="T8" t="n">
-        <v>73518.2</v>
+        <v>65884.36666666667</v>
       </c>
       <c r="U8" t="n">
-        <v>16954.42</v>
+        <v>14485.34333333333</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1379.234643333333</v>
+        <v>1471.535181218638</v>
       </c>
       <c r="B9" t="n">
-        <v>364.1366666666667</v>
+        <v>398.0820788530465</v>
       </c>
       <c r="C9" t="n">
-        <v>215.8333333333333</v>
+        <v>244.225376344086</v>
       </c>
       <c r="D9" t="n">
-        <v>11</v>
+        <v>11.08333333333333</v>
       </c>
       <c r="E9" t="n">
-        <v>4.3</v>
+        <v>3.808888888888889</v>
       </c>
       <c r="F9" t="n">
-        <v>11.18</v>
+        <v>15.92666666666667</v>
       </c>
       <c r="G9" t="n">
-        <v>2075.974646666667</v>
+        <v>2200.957183655914</v>
       </c>
       <c r="H9" t="n">
-        <v>34.4</v>
+        <v>34.5</v>
       </c>
       <c r="I9" t="n">
-        <v>93.45333333333333</v>
+        <v>97.89505376344086</v>
       </c>
       <c r="J9" t="n">
-        <v>9.908494076923077</v>
+        <v>9.797889828555501</v>
       </c>
       <c r="K9" t="n">
-        <v>46.02</v>
+        <v>74.05</v>
       </c>
       <c r="L9" t="n">
-        <v>244.2403333333333</v>
+        <v>251.3184695340502</v>
       </c>
       <c r="M9" t="n">
-        <v>193.4973</v>
+        <v>204.9377089605735</v>
       </c>
       <c r="N9" t="n">
-        <v>1.146333333333333</v>
+        <v>1.906</v>
       </c>
       <c r="O9" t="n">
-        <v>1.28</v>
+        <v>0.91</v>
       </c>
       <c r="P9" t="n">
         <v>0</v>
       </c>
       <c r="Q9" t="n">
-        <v>100.024757682087</v>
+        <v>100.6185806839007</v>
       </c>
       <c r="R9" t="n">
-        <v>121.4003333333333</v>
+        <v>125.0281146953405</v>
       </c>
       <c r="S9" t="n">
-        <v>100.1475666666667</v>
+        <v>103.4573125448029</v>
       </c>
       <c r="T9" t="n">
-        <v>61363.8</v>
+        <v>68361.42939068101</v>
       </c>
       <c r="U9" t="n">
-        <v>13197.58333333333</v>
+        <v>13960.94917562724</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1620.456493333333</v>
+        <v>1580.510146666667</v>
       </c>
       <c r="B10" t="n">
-        <v>536.7552000000001</v>
+        <v>542.1844333333333</v>
       </c>
       <c r="C10" t="n">
-        <v>417.4457</v>
+        <v>381.8903</v>
       </c>
       <c r="D10" t="n">
-        <v>17.16</v>
+        <v>15.97</v>
       </c>
       <c r="E10" t="n">
-        <v>4.603333333333333</v>
+        <v>5.416666666666667</v>
       </c>
       <c r="F10" t="n">
-        <v>23.14</v>
+        <v>15.83</v>
       </c>
       <c r="G10" t="n">
-        <v>2417.547413333333</v>
+        <v>2448.47103</v>
       </c>
       <c r="H10" t="n">
         <v>34.8</v>
       </c>
       <c r="I10" t="n">
-        <v>71.73666666666666</v>
+        <v>81.34333333333333</v>
       </c>
       <c r="J10" t="n">
-        <v>9.318259489130435</v>
+        <v>9.20270443956044</v>
       </c>
       <c r="K10" t="n">
-        <v>75.22</v>
+        <v>73.52</v>
       </c>
       <c r="L10" t="n">
-        <v>276.5108</v>
+        <v>272.1430333333333</v>
       </c>
       <c r="M10" t="n">
-        <v>273.6442</v>
+        <v>265.4335</v>
       </c>
       <c r="N10" t="n">
-        <v>0.08</v>
+        <v>0.09933333333333333</v>
       </c>
       <c r="O10" t="n">
-        <v>1.48</v>
+        <v>1.4</v>
       </c>
       <c r="P10" t="n">
         <v>0</v>
       </c>
       <c r="Q10" t="n">
-        <v>100.3052101638742</v>
+        <v>100.5441661244718</v>
       </c>
       <c r="R10" t="n">
-        <v>129.8516666666667</v>
+        <v>127.9216666666667</v>
       </c>
       <c r="S10" t="n">
-        <v>101.3098533333333</v>
+        <v>100.84973</v>
       </c>
       <c r="T10" t="n">
-        <v>70587.53333333334</v>
+        <v>68643.26666666666</v>
       </c>
       <c r="U10" t="n">
-        <v>16302.14666666667</v>
+        <v>15814.47</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1554.142806451613</v>
+        <v>1575.50846</v>
       </c>
       <c r="B11" t="n">
-        <v>338.4935483870968</v>
+        <v>363.19</v>
       </c>
       <c r="C11" t="n">
-        <v>204.8903225806451</v>
+        <v>206.5966666666667</v>
       </c>
       <c r="D11" t="n">
-        <v>29.19</v>
+        <v>15.37</v>
       </c>
       <c r="E11" t="n">
-        <v>14.36774193548387</v>
+        <v>3.596666666666667</v>
       </c>
       <c r="F11" t="n">
-        <v>53.54</v>
+        <v>16.24</v>
       </c>
       <c r="G11" t="n">
-        <v>2906.205274193548</v>
+        <v>2369.373433333333</v>
       </c>
       <c r="H11" t="n">
-        <v>34.19677419354839</v>
+        <v>34.4</v>
       </c>
       <c r="I11" t="n">
-        <v>72.35806451612903</v>
+        <v>95.42333333333333</v>
       </c>
       <c r="J11" t="n">
-        <v>8.863368769230769</v>
+        <v>9.935092630434783</v>
       </c>
       <c r="K11" t="n">
-        <v>20.51</v>
+        <v>54.09</v>
       </c>
       <c r="L11" t="n">
-        <v>256.1608064516129</v>
+        <v>257.2813666666667</v>
       </c>
       <c r="M11" t="n">
-        <v>217.2059677419355</v>
+        <v>212.0108666666667</v>
       </c>
       <c r="N11" t="n">
-        <v>0.06935483870967751</v>
+        <v>1.837</v>
       </c>
       <c r="O11" t="n">
-        <v>0.59</v>
+        <v>-0.2</v>
       </c>
       <c r="P11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q11" t="n">
-        <v>93.34563685915909</v>
+        <v>99.22913027324101</v>
       </c>
       <c r="R11" t="n">
-        <v>115.9635483870968</v>
+        <v>129.0736666666667</v>
       </c>
       <c r="S11" t="n">
-        <v>85.37563225806451</v>
+        <v>101.8042166666667</v>
       </c>
       <c r="T11" t="n">
-        <v>55711.77419354839</v>
+        <v>65206.86666666667</v>
       </c>
       <c r="U11" t="n">
-        <v>12077.94193548387</v>
+        <v>14606.46</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1526.926783870968</v>
+        <v>1620.456493333333</v>
       </c>
       <c r="B12" t="n">
-        <v>394.3451612903226</v>
+        <v>536.7552000000001</v>
       </c>
       <c r="C12" t="n">
-        <v>234.1483870967742</v>
+        <v>417.4457</v>
       </c>
       <c r="D12" t="n">
-        <v>10.06666666666667</v>
+        <v>17.16</v>
       </c>
       <c r="E12" t="n">
-        <v>3.606451612903226</v>
+        <v>4.603333333333333</v>
       </c>
       <c r="F12" t="n">
-        <v>13.50333333333333</v>
+        <v>23.14</v>
       </c>
       <c r="G12" t="n">
-        <v>2325.921609677419</v>
+        <v>2417.547413333333</v>
       </c>
       <c r="H12" t="n">
-        <v>34.40322580645161</v>
+        <v>34.8</v>
       </c>
       <c r="I12" t="n">
-        <v>97.23870967741935</v>
+        <v>71.73666666666666</v>
       </c>
       <c r="J12" t="n">
-        <v>9.9055614</v>
+        <v>9.318259489130435</v>
       </c>
       <c r="K12" t="n">
-        <v>61.12333333333333</v>
+        <v>75.22</v>
       </c>
       <c r="L12" t="n">
-        <v>255.1342903225807</v>
+        <v>276.5108</v>
       </c>
       <c r="M12" t="n">
-        <v>207.6672903225807</v>
+        <v>273.6442</v>
       </c>
       <c r="N12" t="n">
-        <v>2.419677419354838</v>
+        <v>0.08</v>
       </c>
       <c r="O12" t="n">
-        <v>0.04333333333333333</v>
+        <v>1.48</v>
       </c>
       <c r="P12" t="n">
         <v>0</v>
       </c>
       <c r="Q12" t="n">
-        <v>99.57553045249306</v>
+        <v>100.3052101638742</v>
       </c>
       <c r="R12" t="n">
-        <v>127.6161290322581</v>
+        <v>129.8516666666667</v>
       </c>
       <c r="S12" t="n">
-        <v>102.3992903225806</v>
+        <v>101.3098533333333</v>
       </c>
       <c r="T12" t="n">
-        <v>67056.6129032258</v>
+        <v>70587.53333333334</v>
       </c>
       <c r="U12" t="n">
-        <v>14326.56129032258</v>
+        <v>16302.14666666667</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1575.50846</v>
+        <v>1759.5398</v>
       </c>
       <c r="B13" t="n">
-        <v>363.19</v>
+        <v>542.649</v>
       </c>
       <c r="C13" t="n">
-        <v>206.5966666666667</v>
+        <v>412.865</v>
       </c>
       <c r="D13" t="n">
-        <v>15.37</v>
+        <v>19.61</v>
       </c>
       <c r="E13" t="n">
-        <v>3.596666666666667</v>
+        <v>3.6</v>
       </c>
       <c r="F13" t="n">
-        <v>16.24</v>
+        <v>28.71</v>
       </c>
       <c r="G13" t="n">
-        <v>2369.373433333333</v>
+        <v>2661.893</v>
       </c>
       <c r="H13" t="n">
-        <v>34.4</v>
+        <v>34.5</v>
       </c>
       <c r="I13" t="n">
-        <v>95.42333333333333</v>
+        <v>58.85333333333333</v>
       </c>
       <c r="J13" t="n">
-        <v>9.935092630434783</v>
+        <v>9.516867326086956</v>
       </c>
       <c r="K13" t="n">
-        <v>54.09</v>
+        <v>107.76</v>
       </c>
       <c r="L13" t="n">
-        <v>257.2813666666667</v>
+        <v>295.328</v>
       </c>
       <c r="M13" t="n">
-        <v>212.0108666666667</v>
+        <v>300.845</v>
       </c>
       <c r="N13" t="n">
-        <v>1.837</v>
+        <v>1.21</v>
       </c>
       <c r="O13" t="n">
-        <v>-0.2</v>
+        <v>1.26</v>
       </c>
       <c r="P13" t="n">
         <v>0</v>
       </c>
       <c r="Q13" t="n">
-        <v>99.22913027324101</v>
+        <v>99.4414473129178</v>
       </c>
       <c r="R13" t="n">
-        <v>129.0736666666667</v>
+        <v>134.1606666666667</v>
       </c>
       <c r="S13" t="n">
-        <v>101.8042166666667</v>
+        <v>104.3648</v>
       </c>
       <c r="T13" t="n">
-        <v>65206.86666666667</v>
+        <v>73518.2</v>
       </c>
       <c r="U13" t="n">
-        <v>14606.46</v>
+        <v>16954.42</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1407.679989390681</v>
+        <v>1379.234643333333</v>
       </c>
       <c r="B14" t="n">
-        <v>398.6220071684588</v>
+        <v>364.1366666666667</v>
       </c>
       <c r="C14" t="n">
-        <v>211.6576344086021</v>
+        <v>215.8333333333333</v>
       </c>
       <c r="D14" t="n">
-        <v>11.75333333333333</v>
+        <v>11</v>
       </c>
       <c r="E14" t="n">
-        <v>4.204444444444444</v>
+        <v>4.3</v>
       </c>
       <c r="F14" t="n">
-        <v>9.49</v>
+        <v>11.18</v>
       </c>
       <c r="G14" t="n">
-        <v>2111.770228530466</v>
+        <v>2075.974646666667</v>
       </c>
       <c r="H14" t="n">
-        <v>34.39663082437276</v>
+        <v>34.4</v>
       </c>
       <c r="I14" t="n">
-        <v>100.4274551971326</v>
+        <v>93.45333333333333</v>
       </c>
       <c r="J14" t="n">
-        <v>9.913020010869564</v>
+        <v>9.908494076923077</v>
       </c>
       <c r="K14" t="n">
-        <v>51.31</v>
+        <v>46.02</v>
       </c>
       <c r="L14" t="n">
-        <v>246.6245863799283</v>
+        <v>244.2403333333333</v>
       </c>
       <c r="M14" t="n">
-        <v>195.0992143369176</v>
+        <v>193.4973</v>
       </c>
       <c r="N14" t="n">
-        <v>1.15010752688172</v>
+        <v>1.146333333333333</v>
       </c>
       <c r="O14" t="n">
-        <v>1.29</v>
+        <v>1.28</v>
       </c>
       <c r="P14" t="n">
         <v>0</v>
       </c>
       <c r="Q14" t="n">
-        <v>100.2700716578218</v>
+        <v>100.024757682087</v>
       </c>
       <c r="R14" t="n">
-        <v>122.2105663082437</v>
+        <v>121.4003333333333</v>
       </c>
       <c r="S14" t="n">
-        <v>100.9862233691756</v>
+        <v>100.1475666666667</v>
       </c>
       <c r="T14" t="n">
-        <v>63953.99569892474</v>
+        <v>61363.8</v>
       </c>
       <c r="U14" t="n">
-        <v>13394.56494623656</v>
+        <v>13197.58333333333</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1505.030806451613</v>
+        <v>1524.761677419355</v>
       </c>
       <c r="B15" t="n">
-        <v>371.2516129032258</v>
+        <v>458.1193548387097</v>
       </c>
       <c r="C15" t="n">
-        <v>240.5741935483871</v>
+        <v>250.1516129032258</v>
       </c>
       <c r="D15" t="n">
-        <v>13.48</v>
+        <v>20.79</v>
       </c>
       <c r="E15" t="n">
-        <v>3.996774193548387</v>
+        <v>6.409677419354839</v>
       </c>
       <c r="F15" t="n">
-        <v>25.42</v>
+        <v>22.75</v>
       </c>
       <c r="G15" t="n">
-        <v>2322.726619354838</v>
+        <v>2569.302306451613</v>
       </c>
       <c r="H15" t="n">
-        <v>34.5</v>
+        <v>34.99032258064516</v>
       </c>
       <c r="I15" t="n">
-        <v>91.42903225806452</v>
+        <v>79.05483870967743</v>
       </c>
       <c r="J15" t="n">
-        <v>9.845238065217391</v>
+        <v>8.395245293478261</v>
       </c>
       <c r="K15" t="n">
-        <v>45.846</v>
+        <v>48.35</v>
       </c>
       <c r="L15" t="n">
-        <v>252.4726129032258</v>
+        <v>262.1794838709677</v>
       </c>
       <c r="M15" t="n">
-        <v>204.2487741935484</v>
+        <v>236.4399032258065</v>
       </c>
       <c r="N15" t="n">
-        <v>2.395806451612903</v>
+        <v>0.09</v>
       </c>
       <c r="O15" t="n">
-        <v>0.24</v>
+        <v>0.84</v>
       </c>
       <c r="P15" t="n">
         <v>0</v>
       </c>
       <c r="Q15" t="n">
-        <v>99.82778111835155</v>
+        <v>99.79939459335134</v>
       </c>
       <c r="R15" t="n">
-        <v>126.6096774193548</v>
+        <v>124.2593548387097</v>
       </c>
       <c r="S15" t="n">
-        <v>103.2877741935484</v>
+        <v>99.22816129032257</v>
       </c>
       <c r="T15" t="n">
-        <v>67066.87096774194</v>
+        <v>64724</v>
       </c>
       <c r="U15" t="n">
-        <v>14102.66451612903</v>
+        <v>14842.79032258064</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1459.674851774193</v>
+        <v>1726.708025806452</v>
       </c>
       <c r="B16" t="n">
-        <v>406.9417204301075</v>
+        <v>580.5684838709677</v>
       </c>
       <c r="C16" t="n">
-        <v>233.862311827957</v>
+        <v>405.3624193548387</v>
       </c>
       <c r="D16" t="n">
-        <v>11.96</v>
+        <v>20.25</v>
       </c>
       <c r="E16" t="n">
-        <v>3.996666666666667</v>
+        <v>3.6</v>
       </c>
       <c r="F16" t="n">
-        <v>21.795</v>
+        <v>20.56</v>
       </c>
       <c r="G16" t="n">
-        <v>2161.494655860215</v>
+        <v>2560.214683870968</v>
       </c>
       <c r="H16" t="n">
-        <v>34.5</v>
+        <v>34.6</v>
       </c>
       <c r="I16" t="n">
-        <v>98.91247311827956</v>
+        <v>65.01290322580645</v>
       </c>
       <c r="J16" t="n">
-        <v>9.795628748168497</v>
+        <v>9.516867326086956</v>
       </c>
       <c r="K16" t="n">
-        <v>63.96</v>
+        <v>100.53</v>
       </c>
       <c r="L16" t="n">
-        <v>250.1292112903226</v>
+        <v>288.6321935483871</v>
       </c>
       <c r="M16" t="n">
-        <v>200.5677784946236</v>
+        <v>300.6474516129032</v>
       </c>
       <c r="N16" t="n">
-        <v>1.681456989247312</v>
+        <v>0.3258064516129032</v>
       </c>
       <c r="O16" t="n">
-        <v>0.985</v>
+        <v>1.8</v>
       </c>
       <c r="P16" t="n">
         <v>0</v>
       </c>
       <c r="Q16" t="n">
-        <v>100.6920865385476</v>
+        <v>99.72129721501773</v>
       </c>
       <c r="R16" t="n">
-        <v>124.0734677419355</v>
+        <v>133.7270967741935</v>
       </c>
       <c r="S16" t="n">
-        <v>103.3620803763441</v>
+        <v>104.4967935483871</v>
       </c>
       <c r="T16" t="n">
-        <v>65399.39462365591</v>
+        <v>73106.67741935483</v>
       </c>
       <c r="U16" t="n">
-        <v>13806.2676344086</v>
+        <v>16920.90967741936</v>
       </c>
     </row>
     <row r="17">
@@ -3319,327 +3869,327 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1726.708025806452</v>
+        <v>1518.70469</v>
       </c>
       <c r="B18" t="n">
-        <v>580.5684838709677</v>
+        <v>396.4766666666667</v>
       </c>
       <c r="C18" t="n">
-        <v>405.3624193548387</v>
+        <v>207.3266666666667</v>
       </c>
       <c r="D18" t="n">
-        <v>20.25</v>
+        <v>22.07</v>
       </c>
       <c r="E18" t="n">
-        <v>3.6</v>
+        <v>6.933333333333334</v>
       </c>
       <c r="F18" t="n">
-        <v>20.56</v>
+        <v>26.37</v>
       </c>
       <c r="G18" t="n">
-        <v>2560.214683870968</v>
+        <v>2698.391866666667</v>
       </c>
       <c r="H18" t="n">
-        <v>34.6</v>
+        <v>34.89666666666667</v>
       </c>
       <c r="I18" t="n">
-        <v>65.01290322580645</v>
+        <v>81.75333333333333</v>
       </c>
       <c r="J18" t="n">
-        <v>9.516867326086956</v>
+        <v>9.402214543478262</v>
       </c>
       <c r="K18" t="n">
-        <v>100.53</v>
+        <v>40.05</v>
       </c>
       <c r="L18" t="n">
-        <v>288.6321935483871</v>
+        <v>260.3466</v>
       </c>
       <c r="M18" t="n">
-        <v>300.6474516129032</v>
+        <v>229.7583333333334</v>
       </c>
       <c r="N18" t="n">
-        <v>0.3258064516129032</v>
+        <v>0.09</v>
       </c>
       <c r="O18" t="n">
-        <v>1.8</v>
+        <v>0.59</v>
       </c>
       <c r="P18" t="n">
         <v>0</v>
       </c>
       <c r="Q18" t="n">
-        <v>99.72129721501773</v>
+        <v>98.79102009760062</v>
       </c>
       <c r="R18" t="n">
-        <v>133.7270967741935</v>
+        <v>122.8773333333333</v>
       </c>
       <c r="S18" t="n">
-        <v>104.4967935483871</v>
+        <v>96.79987</v>
       </c>
       <c r="T18" t="n">
-        <v>73106.67741935483</v>
+        <v>62779.6</v>
       </c>
       <c r="U18" t="n">
-        <v>16920.90967741936</v>
+        <v>14543.85666666667</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1524.761677419355</v>
+        <v>1530.413548387097</v>
       </c>
       <c r="B19" t="n">
-        <v>458.1193548387097</v>
+        <v>504.5</v>
       </c>
       <c r="C19" t="n">
-        <v>250.1516129032258</v>
+        <v>320.3612903225807</v>
       </c>
       <c r="D19" t="n">
-        <v>20.79</v>
+        <v>17.07</v>
       </c>
       <c r="E19" t="n">
-        <v>6.409677419354839</v>
+        <v>6</v>
       </c>
       <c r="F19" t="n">
-        <v>22.75</v>
+        <v>19.4</v>
       </c>
       <c r="G19" t="n">
-        <v>2569.302306451613</v>
+        <v>2552.336158064516</v>
       </c>
       <c r="H19" t="n">
-        <v>34.99032258064516</v>
+        <v>34.9</v>
       </c>
       <c r="I19" t="n">
-        <v>79.05483870967743</v>
+        <v>88.19032258064516</v>
       </c>
       <c r="J19" t="n">
-        <v>8.395245293478261</v>
+        <v>9.101889566666667</v>
       </c>
       <c r="K19" t="n">
-        <v>48.35</v>
+        <v>59.19</v>
       </c>
       <c r="L19" t="n">
-        <v>262.1794838709677</v>
+        <v>266.6721935483871</v>
       </c>
       <c r="M19" t="n">
-        <v>236.4399032258065</v>
+        <v>249.7142580645161</v>
       </c>
       <c r="N19" t="n">
-        <v>0.09</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="O19" t="n">
-        <v>0.84</v>
+        <v>1.71</v>
       </c>
       <c r="P19" t="n">
         <v>0</v>
       </c>
       <c r="Q19" t="n">
-        <v>99.79939459335134</v>
+        <v>100.5973786748587</v>
       </c>
       <c r="R19" t="n">
-        <v>124.2593548387097</v>
+        <v>125.9677419354839</v>
       </c>
       <c r="S19" t="n">
-        <v>99.22816129032257</v>
+        <v>99.01935806451614</v>
       </c>
       <c r="T19" t="n">
-        <v>64724</v>
+        <v>67888.25806451614</v>
       </c>
       <c r="U19" t="n">
-        <v>14842.79032258064</v>
+        <v>15613.54516129032</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1433.161535483871</v>
+        <v>1505.030806451613</v>
       </c>
       <c r="B20" t="n">
-        <v>410.1193548387097</v>
+        <v>371.2516129032258</v>
       </c>
       <c r="C20" t="n">
-        <v>217.4451612903226</v>
+        <v>240.5741935483871</v>
       </c>
       <c r="D20" t="n">
-        <v>11.46</v>
+        <v>13.48</v>
       </c>
       <c r="E20" t="n">
-        <v>4.006451612903225</v>
+        <v>3.996774193548387</v>
       </c>
       <c r="F20" t="n">
-        <v>10.405</v>
+        <v>25.42</v>
       </c>
       <c r="G20" t="n">
-        <v>2107.725608064516</v>
+        <v>2322.726619354838</v>
       </c>
       <c r="H20" t="n">
-        <v>34.40645161290323</v>
+        <v>34.5</v>
       </c>
       <c r="I20" t="n">
-        <v>95.7741935483871</v>
+        <v>91.42903225806452</v>
       </c>
       <c r="J20" t="n">
-        <v>9.846498242149758</v>
+        <v>9.845238065217391</v>
       </c>
       <c r="K20" t="n">
-        <v>60.415</v>
+        <v>45.846</v>
       </c>
       <c r="L20" t="n">
-        <v>248.7088387096774</v>
+        <v>252.4726129032258</v>
       </c>
       <c r="M20" t="n">
-        <v>196.1336774193548</v>
+        <v>204.2487741935484</v>
       </c>
       <c r="N20" t="n">
-        <v>1.404838709677419</v>
+        <v>2.395806451612903</v>
       </c>
       <c r="O20" t="n">
-        <v>1.015</v>
+        <v>0.24</v>
       </c>
       <c r="P20" t="n">
         <v>0</v>
       </c>
       <c r="Q20" t="n">
-        <v>100.5199462359304</v>
+        <v>99.82778111835155</v>
       </c>
       <c r="R20" t="n">
-        <v>123.0925806451613</v>
+        <v>126.6096774193548</v>
       </c>
       <c r="S20" t="n">
-        <v>101.3529064516129</v>
+        <v>103.2877741935484</v>
       </c>
       <c r="T20" t="n">
-        <v>63835.80645161291</v>
+        <v>67066.87096774194</v>
       </c>
       <c r="U20" t="n">
-        <v>13619.81290322581</v>
+        <v>14102.66451612903</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1530.413548387097</v>
+        <v>1518.463696666667</v>
       </c>
       <c r="B21" t="n">
-        <v>504.5</v>
+        <v>382.71</v>
       </c>
       <c r="C21" t="n">
-        <v>320.3612903225807</v>
+        <v>200.9866666666667</v>
       </c>
       <c r="D21" t="n">
-        <v>17.07</v>
+        <v>19.65</v>
       </c>
       <c r="E21" t="n">
-        <v>6</v>
+        <v>10.22666666666667</v>
       </c>
       <c r="F21" t="n">
-        <v>19.4</v>
+        <v>30.43</v>
       </c>
       <c r="G21" t="n">
-        <v>2552.336158064516</v>
+        <v>2858.75815</v>
       </c>
       <c r="H21" t="n">
-        <v>34.9</v>
+        <v>34.6</v>
       </c>
       <c r="I21" t="n">
-        <v>88.19032258064516</v>
+        <v>72.68666666666667</v>
       </c>
       <c r="J21" t="n">
-        <v>9.101889566666667</v>
+        <v>9.193901098901099</v>
       </c>
       <c r="K21" t="n">
-        <v>59.19</v>
+        <v>39.27</v>
       </c>
       <c r="L21" t="n">
-        <v>266.6721935483871</v>
+        <v>258.4988</v>
       </c>
       <c r="M21" t="n">
-        <v>249.7142580645161</v>
+        <v>221.5394333333333</v>
       </c>
       <c r="N21" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.08966666666666666</v>
       </c>
       <c r="O21" t="n">
-        <v>1.71</v>
+        <v>0.5</v>
       </c>
       <c r="P21" t="n">
         <v>0</v>
       </c>
       <c r="Q21" t="n">
-        <v>100.5973786748587</v>
+        <v>97.62538150086982</v>
       </c>
       <c r="R21" t="n">
-        <v>125.9677419354839</v>
+        <v>119.739</v>
       </c>
       <c r="S21" t="n">
-        <v>99.01935806451614</v>
+        <v>95.12751333333333</v>
       </c>
       <c r="T21" t="n">
-        <v>67888.25806451614</v>
+        <v>60043.43333333333</v>
       </c>
       <c r="U21" t="n">
-        <v>15613.54516129032</v>
+        <v>14121.20333333333</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1488.268166666667</v>
+        <v>1526.926783870968</v>
       </c>
       <c r="B22" t="n">
-        <v>376.0766666666667</v>
+        <v>394.3451612903226</v>
       </c>
       <c r="C22" t="n">
-        <v>244.12</v>
+        <v>234.1483870967742</v>
       </c>
       <c r="D22" t="n">
-        <v>10.93333333333333</v>
+        <v>10.06666666666667</v>
       </c>
       <c r="E22" t="n">
-        <v>3.796666666666666</v>
+        <v>3.606451612903226</v>
       </c>
       <c r="F22" t="n">
-        <v>12.04</v>
+        <v>13.50333333333333</v>
       </c>
       <c r="G22" t="n">
-        <v>2247.25593</v>
+        <v>2325.921609677419</v>
       </c>
       <c r="H22" t="n">
-        <v>34.5</v>
+        <v>34.40322580645161</v>
       </c>
       <c r="I22" t="n">
-        <v>98.64999999999999</v>
+        <v>97.23870967741935</v>
       </c>
       <c r="J22" t="n">
-        <v>9.811155195652175</v>
+        <v>9.9055614</v>
       </c>
       <c r="K22" t="n">
-        <v>74.63333333333334</v>
+        <v>61.12333333333333</v>
       </c>
       <c r="L22" t="n">
-        <v>252.8412333333333</v>
+        <v>255.1342903225807</v>
       </c>
       <c r="M22" t="n">
-        <v>205.3912</v>
+        <v>207.6672903225807</v>
       </c>
       <c r="N22" t="n">
-        <v>2.182</v>
+        <v>2.419677419354838</v>
       </c>
       <c r="O22" t="n">
-        <v>0.86</v>
+        <v>0.04333333333333333</v>
       </c>
       <c r="P22" t="n">
         <v>0</v>
       </c>
       <c r="Q22" t="n">
-        <v>100.2896470386735</v>
+        <v>99.57553045249306</v>
       </c>
       <c r="R22" t="n">
-        <v>125.8326666666667</v>
+        <v>127.6161290322581</v>
       </c>
       <c r="S22" t="n">
-        <v>104.0515633333333</v>
+        <v>102.3992903225806</v>
       </c>
       <c r="T22" t="n">
-        <v>67904.2</v>
+        <v>67056.6129032258</v>
       </c>
       <c r="U22" t="n">
-        <v>14116.63666666667</v>
+        <v>14326.56129032258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>